<commit_message>
tach rieng cot kinh do vi do
</commit_message>
<xml_diff>
--- a/Scripts/data/stores_coordinates_case_300.xlsx
+++ b/Scripts/data/stores_coordinates_case_300.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B302"/>
+  <dimension ref="A1:C302"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Coordinates</t>
+          <t>Longitude</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Latitude</t>
         </is>
       </c>
     </row>
@@ -451,10 +456,11 @@
           <t>Cửa Hàng Vlxd Tuấn Mai</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>107.083798,10.34516,0</t>
-        </is>
+      <c r="B2" t="n">
+        <v>107.083798</v>
+      </c>
+      <c r="C2" t="n">
+        <v>10.34516</v>
       </c>
     </row>
     <row r="3">
@@ -463,10 +469,11 @@
           <t>Cửa Hàng Vlxd Huỳnh Nga</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>107.09049,10.36099,0</t>
-        </is>
+      <c r="B3" t="n">
+        <v>107.09049</v>
+      </c>
+      <c r="C3" t="n">
+        <v>10.36099</v>
       </c>
     </row>
     <row r="4">
@@ -475,10 +482,11 @@
           <t>Công Ty Cổ Phần Kinh Doanh Vật Liệu Xây Dựng Số 15 (Office)</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>107.089001,10.373341,0</t>
-        </is>
+      <c r="B4" t="n">
+        <v>107.089001</v>
+      </c>
+      <c r="C4" t="n">
+        <v>10.373341</v>
       </c>
     </row>
     <row r="5">
@@ -487,10 +495,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Đông Thành</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>107.092462,10.362762,0</t>
-        </is>
+      <c r="B5" t="n">
+        <v>107.092462</v>
+      </c>
+      <c r="C5" t="n">
+        <v>10.362762</v>
       </c>
     </row>
     <row r="6">
@@ -499,10 +508,11 @@
           <t>cửa hàng vật liệu xây dựng mạnh phú</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>107.102156,10.375412,0</t>
-        </is>
+      <c r="B6" t="n">
+        <v>107.102156</v>
+      </c>
+      <c r="C6" t="n">
+        <v>10.375412</v>
       </c>
     </row>
     <row r="7">
@@ -511,10 +521,11 @@
           <t>CỬA HÀNG VLXD MẠNH PHÚ MATERIALS</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>107.103123,10.376154,0</t>
-        </is>
+      <c r="B7" t="n">
+        <v>107.103123</v>
+      </c>
+      <c r="C7" t="n">
+        <v>10.376154</v>
       </c>
     </row>
     <row r="8">
@@ -523,10 +534,11 @@
           <t>Cửa Hàng Vlxd An Phát</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>107.091319,10.361738,0</t>
-        </is>
+      <c r="B8" t="n">
+        <v>107.091319</v>
+      </c>
+      <c r="C8" t="n">
+        <v>10.361738</v>
       </c>
     </row>
     <row r="9">
@@ -535,10 +547,11 @@
           <t>Vật liệu Nội Thất Mạnh Phát</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>107.107668,10.378978,0</t>
-        </is>
+      <c r="B9" t="n">
+        <v>107.107668</v>
+      </c>
+      <c r="C9" t="n">
+        <v>10.378978</v>
       </c>
     </row>
     <row r="10">
@@ -547,10 +560,11 @@
           <t>Công ty TNHH Vật Tư Xây Dựng Thẩm</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>107.089926,10.35982,0</t>
-        </is>
+      <c r="B10" t="n">
+        <v>107.089926</v>
+      </c>
+      <c r="C10" t="n">
+        <v>10.35982</v>
       </c>
     </row>
     <row r="11">
@@ -559,10 +573,11 @@
           <t>CỬA HÀNG VẬT LIỆU XÂY DỰNG VIỆT HÀ - Vật Liệu Xây Dựng Chất Lượng Tại Vũng Tàu</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>107.08311,10.356019,0</t>
-        </is>
+      <c r="B11" t="n">
+        <v>107.08311</v>
+      </c>
+      <c r="C11" t="n">
+        <v>10.356019</v>
       </c>
     </row>
     <row r="12">
@@ -571,10 +586,11 @@
           <t>Cửa hàng vật liệu gỗ xây dựng đại duyên</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>107.039614,10.653406,0</t>
-        </is>
+      <c r="B12" t="n">
+        <v>107.039614</v>
+      </c>
+      <c r="C12" t="n">
+        <v>10.653406</v>
       </c>
     </row>
     <row r="13">
@@ -583,10 +599,11 @@
           <t>Cửa Hàng Vlxd Đại Thành</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>107.197005,10.500072,0</t>
-        </is>
+      <c r="B13" t="n">
+        <v>107.197005</v>
+      </c>
+      <c r="C13" t="n">
+        <v>10.500072</v>
       </c>
     </row>
     <row r="14">
@@ -595,10 +612,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Hiệp Thành</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>107.045426,10.657472,0</t>
-        </is>
+      <c r="B14" t="n">
+        <v>107.045426</v>
+      </c>
+      <c r="C14" t="n">
+        <v>10.657472</v>
       </c>
     </row>
     <row r="15">
@@ -607,10 +625,11 @@
           <t>Công Ty TNHH Vật Liệu Xây Dựng Bà Rịa</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>107.152436,10.504947,0</t>
-        </is>
+      <c r="B15" t="n">
+        <v>107.152436</v>
+      </c>
+      <c r="C15" t="n">
+        <v>10.504947</v>
       </c>
     </row>
     <row r="16">
@@ -619,10 +638,11 @@
           <t>Vật liệu xây dựng Thể</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>107.271092,10.490306,0</t>
-        </is>
+      <c r="B16" t="n">
+        <v>107.271092</v>
+      </c>
+      <c r="C16" t="n">
+        <v>10.490306</v>
       </c>
     </row>
     <row r="17">
@@ -631,10 +651,11 @@
           <t>Vật Liệu Xây Dựng Diệu Loan</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>107.220591,10.575376,0</t>
-        </is>
+      <c r="B17" t="n">
+        <v>107.220591</v>
+      </c>
+      <c r="C17" t="n">
+        <v>10.575376</v>
       </c>
     </row>
     <row r="18">
@@ -643,10 +664,11 @@
           <t>Cửa Hàng VLXD Điệp</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>107.169178,10.494,0</t>
-        </is>
+      <c r="B18" t="n">
+        <v>107.169178</v>
+      </c>
+      <c r="C18" t="n">
+        <v>10.494</v>
       </c>
     </row>
     <row r="19">
@@ -655,10 +677,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Thanh Xuân</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>107.167941,10.520952,0</t>
-        </is>
+      <c r="B19" t="n">
+        <v>107.167941</v>
+      </c>
+      <c r="C19" t="n">
+        <v>10.520952</v>
       </c>
     </row>
     <row r="20">
@@ -667,10 +690,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Võ Văn Tài</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>107.171011,10.499273,0</t>
-        </is>
+      <c r="B20" t="n">
+        <v>107.171011</v>
+      </c>
+      <c r="C20" t="n">
+        <v>10.499273</v>
       </c>
     </row>
     <row r="21">
@@ -679,10 +703,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Nguyễn Thị Xuyên</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>107.188963,10.490189,0</t>
-        </is>
+      <c r="B21" t="n">
+        <v>107.188963</v>
+      </c>
+      <c r="C21" t="n">
+        <v>10.490189</v>
       </c>
     </row>
     <row r="22">
@@ -691,10 +716,11 @@
           <t>Cửa Hàng Vlxd Trinh Dũng</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>107.209527,10.408279,0</t>
-        </is>
+      <c r="B22" t="n">
+        <v>107.209527</v>
+      </c>
+      <c r="C22" t="n">
+        <v>10.408279</v>
       </c>
     </row>
     <row r="23">
@@ -703,10 +729,11 @@
           <t>CÔNG TY TNHH TÂN LONG PHÚ MỸ - Đại Lý Vật Tư Điện Nước Bảo Hộ Lao Động</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>107.073832,10.469644,0</t>
-        </is>
+      <c r="B23" t="n">
+        <v>107.073832</v>
+      </c>
+      <c r="C23" t="n">
+        <v>10.469644</v>
       </c>
     </row>
     <row r="24">
@@ -715,10 +742,11 @@
           <t>Vật Liệu Xây Dựng - Trang Trí Nội Thất Lương Phương Nam</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>107.21959,10.411207,0</t>
-        </is>
+      <c r="B24" t="n">
+        <v>107.21959</v>
+      </c>
+      <c r="C24" t="n">
+        <v>10.411207</v>
       </c>
     </row>
     <row r="25">
@@ -727,10 +755,11 @@
           <t>Công Ty TNHH Minh Hiệp</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>107.234033,10.394698,0</t>
-        </is>
+      <c r="B25" t="n">
+        <v>107.234033</v>
+      </c>
+      <c r="C25" t="n">
+        <v>10.394698</v>
       </c>
     </row>
     <row r="26">
@@ -739,10 +768,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Nam Việt</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>107.289726,10.437958,0</t>
-        </is>
+      <c r="B26" t="n">
+        <v>107.289726</v>
+      </c>
+      <c r="C26" t="n">
+        <v>10.437958</v>
       </c>
     </row>
     <row r="27">
@@ -751,10 +781,11 @@
           <t>Vlxd &amp; Trang Trí Ngoại Thất Thủy Long</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>107.228903,10.425735,0</t>
-        </is>
+      <c r="B27" t="n">
+        <v>107.228903</v>
+      </c>
+      <c r="C27" t="n">
+        <v>10.425735</v>
       </c>
     </row>
     <row r="28">
@@ -763,10 +794,11 @@
           <t>Công Ty TNHH Vật Liệu Xây Dựng Long Vũ</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>107.093307,10.60677,0</t>
-        </is>
+      <c r="B28" t="n">
+        <v>107.093307</v>
+      </c>
+      <c r="C28" t="n">
+        <v>10.60677</v>
       </c>
     </row>
     <row r="29">
@@ -775,10 +807,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Thắng Lợi</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>107.237639,10.397583,0</t>
-        </is>
+      <c r="B29" t="n">
+        <v>107.237639</v>
+      </c>
+      <c r="C29" t="n">
+        <v>10.397583</v>
       </c>
     </row>
     <row r="30">
@@ -787,10 +820,11 @@
           <t>Cửa Hàng Vlxd Lộc Phát</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>107.197677,10.485748,0</t>
-        </is>
+      <c r="B30" t="n">
+        <v>107.197677</v>
+      </c>
+      <c r="C30" t="n">
+        <v>10.485748</v>
       </c>
     </row>
     <row r="31">
@@ -799,10 +833,11 @@
           <t>Vật Liệu Xây Dựng Thành Phát</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>107.223022,10.415907,0</t>
-        </is>
+      <c r="B31" t="n">
+        <v>107.223022</v>
+      </c>
+      <c r="C31" t="n">
+        <v>10.415907</v>
       </c>
     </row>
     <row r="32">
@@ -811,10 +846,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Hồng Phát</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>107.27652,10.499033,0</t>
-        </is>
+      <c r="B32" t="n">
+        <v>107.27652</v>
+      </c>
+      <c r="C32" t="n">
+        <v>10.499033</v>
       </c>
     </row>
     <row r="33">
@@ -823,10 +859,11 @@
           <t>Cửa Hàng Điện Nước Huỳnh Hiếu</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>107.242556,10.537951,0</t>
-        </is>
+      <c r="B33" t="n">
+        <v>107.242556</v>
+      </c>
+      <c r="C33" t="n">
+        <v>10.537951</v>
       </c>
     </row>
     <row r="34">
@@ -835,10 +872,11 @@
           <t>Vật liệu xây dựng Thể</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>107.271092,10.490306,0</t>
-        </is>
+      <c r="B34" t="n">
+        <v>107.271092</v>
+      </c>
+      <c r="C34" t="n">
+        <v>10.490306</v>
       </c>
     </row>
     <row r="35">
@@ -847,10 +885,11 @@
           <t>Vật liệu xây dựng Xuân Phát</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>107.271245,10.49026,0</t>
-        </is>
+      <c r="B35" t="n">
+        <v>107.271245</v>
+      </c>
+      <c r="C35" t="n">
+        <v>10.49026</v>
       </c>
     </row>
     <row r="36">
@@ -859,10 +898,11 @@
           <t>Gạch men Hoàng Phương</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>107.262643,10.487833,0</t>
-        </is>
+      <c r="B36" t="n">
+        <v>107.262643</v>
+      </c>
+      <c r="C36" t="n">
+        <v>10.487833</v>
       </c>
     </row>
     <row r="37">
@@ -871,10 +911,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Phước Trung</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>107.283172,10.496277,0</t>
-        </is>
+      <c r="B37" t="n">
+        <v>107.283172</v>
+      </c>
+      <c r="C37" t="n">
+        <v>10.496277</v>
       </c>
     </row>
     <row r="38">
@@ -883,10 +924,11 @@
           <t>Vật liệu xây dựng Kim Chuộng</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>107.270895,10.489947,0</t>
-        </is>
+      <c r="B38" t="n">
+        <v>107.270895</v>
+      </c>
+      <c r="C38" t="n">
+        <v>10.489947</v>
       </c>
     </row>
     <row r="39">
@@ -895,10 +937,11 @@
           <t>Trung Tâm Vlxd Trang Trí Nội Thất Tân thuận</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>107.265314,10.488023,0</t>
-        </is>
+      <c r="B39" t="n">
+        <v>107.265314</v>
+      </c>
+      <c r="C39" t="n">
+        <v>10.488023</v>
       </c>
     </row>
     <row r="40">
@@ -907,10 +950,11 @@
           <t>Cửa hàng vật liệu xây dựng Kim Chuộng</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>107.261745,10.488977,0</t>
-        </is>
+      <c r="B40" t="n">
+        <v>107.261745</v>
+      </c>
+      <c r="C40" t="n">
+        <v>10.488977</v>
       </c>
     </row>
     <row r="41">
@@ -919,10 +963,11 @@
           <t>Cửa Hàng Vlxd Minh Trí</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>107.266542,10.541085,0</t>
-        </is>
+      <c r="B41" t="n">
+        <v>107.266542</v>
+      </c>
+      <c r="C41" t="n">
+        <v>10.541085</v>
       </c>
     </row>
     <row r="42">
@@ -931,10 +976,11 @@
           <t>Cửa Hàng Vlxd Ba Phương</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>107.230189,10.468438,0</t>
-        </is>
+      <c r="B42" t="n">
+        <v>107.230189</v>
+      </c>
+      <c r="C42" t="n">
+        <v>10.468438</v>
       </c>
     </row>
     <row r="43">
@@ -943,10 +989,11 @@
           <t>Cửa Hàng Vlxd Tím</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>107.23159,10.528854,0</t>
-        </is>
+      <c r="B43" t="n">
+        <v>107.23159</v>
+      </c>
+      <c r="C43" t="n">
+        <v>10.528854</v>
       </c>
     </row>
     <row r="44">
@@ -955,10 +1002,11 @@
           <t>Vật Liệu Xây Dựng Tâm Phát Tài</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>107.290192,10.498843,0</t>
-        </is>
+      <c r="B44" t="n">
+        <v>107.290192</v>
+      </c>
+      <c r="C44" t="n">
+        <v>10.498843</v>
       </c>
     </row>
     <row r="45">
@@ -967,10 +1015,11 @@
           <t>Cửa Hàng Vlxd Kến Trúc</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>107.170949,10.495647,0</t>
-        </is>
+      <c r="B45" t="n">
+        <v>107.170949</v>
+      </c>
+      <c r="C45" t="n">
+        <v>10.495647</v>
       </c>
     </row>
     <row r="46">
@@ -979,10 +1028,11 @@
           <t>Cửa Hàng Vlxd Cô Bướm</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>107.231262,10.528482,0</t>
-        </is>
+      <c r="B46" t="n">
+        <v>107.231262</v>
+      </c>
+      <c r="C46" t="n">
+        <v>10.528482</v>
       </c>
     </row>
     <row r="47">
@@ -991,10 +1041,11 @@
           <t>Cơ sở Nhôm Sắt Quy Huỳnh</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>107.24542,10.46164,0</t>
-        </is>
+      <c r="B47" t="n">
+        <v>107.24542</v>
+      </c>
+      <c r="C47" t="n">
+        <v>10.46164</v>
       </c>
     </row>
     <row r="48">
@@ -1003,10 +1054,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Nam Việt</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>107.289726,10.437958,0</t>
-        </is>
+      <c r="B48" t="n">
+        <v>107.289726</v>
+      </c>
+      <c r="C48" t="n">
+        <v>10.437958</v>
       </c>
     </row>
     <row r="49">
@@ -1015,10 +1067,11 @@
           <t>Cửa Hàng Vlxd Thăng Long</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>107.178943,10.496849,0</t>
-        </is>
+      <c r="B49" t="n">
+        <v>107.178943</v>
+      </c>
+      <c r="C49" t="n">
+        <v>10.496849</v>
       </c>
     </row>
     <row r="50">
@@ -1027,10 +1080,11 @@
           <t>Cửa hàng vật liệu xây dựng công minh</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>107.182777,10.492179,0</t>
-        </is>
+      <c r="B50" t="n">
+        <v>107.182777</v>
+      </c>
+      <c r="C50" t="n">
+        <v>10.492179</v>
       </c>
     </row>
     <row r="51">
@@ -1039,10 +1093,11 @@
           <t>TRUNG TÂM VLXD - TRANG TRÍ NỘI THẤT HOÀNG KHÔI</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>107.193321,10.485835,0</t>
-        </is>
+      <c r="B51" t="n">
+        <v>107.193321</v>
+      </c>
+      <c r="C51" t="n">
+        <v>10.485835</v>
       </c>
     </row>
     <row r="52">
@@ -1051,10 +1106,11 @@
           <t>Cửa Hàng Vlxd Kiến Trúc</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>107.163724,10.498605,0</t>
-        </is>
+      <c r="B52" t="n">
+        <v>107.163724</v>
+      </c>
+      <c r="C52" t="n">
+        <v>10.498605</v>
       </c>
     </row>
     <row r="53">
@@ -1063,10 +1119,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Thảo</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>107.20482,10.521311,0</t>
-        </is>
+      <c r="B53" t="n">
+        <v>107.20482</v>
+      </c>
+      <c r="C53" t="n">
+        <v>10.521311</v>
       </c>
     </row>
     <row r="54">
@@ -1075,10 +1132,11 @@
           <t>Vật Liệu Xây Dựng Tỉnh Tâm</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>107.208381,10.570961,0</t>
-        </is>
+      <c r="B54" t="n">
+        <v>107.208381</v>
+      </c>
+      <c r="C54" t="n">
+        <v>10.570961</v>
       </c>
     </row>
     <row r="55">
@@ -1087,10 +1145,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Quang Cường</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>107.229386,10.588057,0</t>
-        </is>
+      <c r="B55" t="n">
+        <v>107.229386</v>
+      </c>
+      <c r="C55" t="n">
+        <v>10.588057</v>
       </c>
     </row>
     <row r="56">
@@ -1099,10 +1158,11 @@
           <t>CỬA HÀNG Trần La Phông HOÀNG PHƯƠNG 3</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>107.211358,10.592591,0</t>
-        </is>
+      <c r="B56" t="n">
+        <v>107.211358</v>
+      </c>
+      <c r="C56" t="n">
+        <v>10.592591</v>
       </c>
     </row>
     <row r="57">
@@ -1111,10 +1171,11 @@
           <t>VLXD ĐẠO THỦY</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>107.3081,10.585334,0</t>
-        </is>
+      <c r="B57" t="n">
+        <v>107.3081</v>
+      </c>
+      <c r="C57" t="n">
+        <v>10.585334</v>
       </c>
     </row>
     <row r="58">
@@ -1123,10 +1184,11 @@
           <t>Vật Liệu Xây Dựng Diệu Loan</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>107.220591,10.575376,0</t>
-        </is>
+      <c r="B58" t="n">
+        <v>107.220591</v>
+      </c>
+      <c r="C58" t="n">
+        <v>10.575376</v>
       </c>
     </row>
     <row r="59">
@@ -1135,10 +1197,11 @@
           <t>Vật liệu xây dựng hổ</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>107.203403,10.602037,0</t>
-        </is>
+      <c r="B59" t="n">
+        <v>107.203403</v>
+      </c>
+      <c r="C59" t="n">
+        <v>10.602037</v>
       </c>
     </row>
     <row r="60">
@@ -1147,10 +1210,11 @@
           <t>Công Ty Trách Nhiệm Hữu Hạn Thương Mại Và Dịch Vụ Công Nghệ Cao Nguyễn</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>107.209525,10.591269,0</t>
-        </is>
+      <c r="B60" t="n">
+        <v>107.209525</v>
+      </c>
+      <c r="C60" t="n">
+        <v>10.591269</v>
       </c>
     </row>
     <row r="61">
@@ -1159,10 +1223,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Liên Chương</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>107.312057,10.582924,0</t>
-        </is>
+      <c r="B61" t="n">
+        <v>107.312057</v>
+      </c>
+      <c r="C61" t="n">
+        <v>10.582924</v>
       </c>
     </row>
     <row r="62">
@@ -1171,10 +1236,11 @@
           <t>VLXD DANH LUYẾN</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>107.225211,10.643967,0</t>
-        </is>
+      <c r="B62" t="n">
+        <v>107.225211</v>
+      </c>
+      <c r="C62" t="n">
+        <v>10.643967</v>
       </c>
     </row>
     <row r="63">
@@ -1183,10 +1249,11 @@
           <t>Trung tâm pha màu SONBOSS Tiên Tiến Phát</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>107.208176,10.591977,0</t>
-        </is>
+      <c r="B63" t="n">
+        <v>107.208176</v>
+      </c>
+      <c r="C63" t="n">
+        <v>10.591977</v>
       </c>
     </row>
     <row r="64">
@@ -1195,10 +1262,11 @@
           <t>Cửa Hàng VLXD Anh Thư</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>107.100867,10.37408,0</t>
-        </is>
+      <c r="B64" t="n">
+        <v>107.100867</v>
+      </c>
+      <c r="C64" t="n">
+        <v>10.37408</v>
       </c>
     </row>
     <row r="65">
@@ -1207,10 +1275,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Hoàng Thu Phương</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>107.114335,10.383671,0</t>
-        </is>
+      <c r="B65" t="n">
+        <v>107.114335</v>
+      </c>
+      <c r="C65" t="n">
+        <v>10.383671</v>
       </c>
     </row>
     <row r="66">
@@ -1219,10 +1288,11 @@
           <t>VLXD HOÀNG MAI</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>107.126075,10.390156,0</t>
-        </is>
+      <c r="B66" t="n">
+        <v>107.126075</v>
+      </c>
+      <c r="C66" t="n">
+        <v>10.390156</v>
       </c>
     </row>
     <row r="67">
@@ -1231,10 +1301,11 @@
           <t>Cửa Hàng Vlxd &amp; Trang Trí Nội Thất Thanh Long</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>107.087178,10.356134,0</t>
-        </is>
+      <c r="B67" t="n">
+        <v>107.087178</v>
+      </c>
+      <c r="C67" t="n">
+        <v>10.356134</v>
       </c>
     </row>
     <row r="68">
@@ -1243,10 +1314,11 @@
           <t>Cửa Hàng VLXD Quang Tuấn</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>107.153983,10.42143,0</t>
-        </is>
+      <c r="B68" t="n">
+        <v>107.153983</v>
+      </c>
+      <c r="C68" t="n">
+        <v>10.42143</v>
       </c>
     </row>
     <row r="69">
@@ -1255,10 +1327,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Tấn Dũng</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>107.146679,10.41034,0</t>
-        </is>
+      <c r="B69" t="n">
+        <v>107.146679</v>
+      </c>
+      <c r="C69" t="n">
+        <v>10.41034</v>
       </c>
     </row>
     <row r="70">
@@ -1267,10 +1340,11 @@
           <t>Cửa Hàng Vlxd Mỹ Đức</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>107.124069,10.389222,0</t>
-        </is>
+      <c r="B70" t="n">
+        <v>107.124069</v>
+      </c>
+      <c r="C70" t="n">
+        <v>10.389222</v>
       </c>
     </row>
     <row r="71">
@@ -1279,10 +1353,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Lê Bá Lương</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>107.103371,10.380116,0</t>
-        </is>
+      <c r="B71" t="n">
+        <v>107.103371</v>
+      </c>
+      <c r="C71" t="n">
+        <v>10.380116</v>
       </c>
     </row>
     <row r="72">
@@ -1291,10 +1366,11 @@
           <t>Cửa Hàng Điện Nước - Thiết Bị Vật Liệu Xây Dựng Minh Thắng</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>107.139878,10.408947,0</t>
-        </is>
+      <c r="B72" t="n">
+        <v>107.139878</v>
+      </c>
+      <c r="C72" t="n">
+        <v>10.408947</v>
       </c>
     </row>
     <row r="73">
@@ -1303,10 +1379,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Thành Công</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>107.167306,10.417058,0</t>
-        </is>
+      <c r="B73" t="n">
+        <v>107.167306</v>
+      </c>
+      <c r="C73" t="n">
+        <v>10.417058</v>
       </c>
     </row>
     <row r="74">
@@ -1315,10 +1392,11 @@
           <t>VLXD Thiên Định</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>107.136394,10.397997,0</t>
-        </is>
+      <c r="B74" t="n">
+        <v>107.136394</v>
+      </c>
+      <c r="C74" t="n">
+        <v>10.397997</v>
       </c>
     </row>
     <row r="75">
@@ -1327,10 +1405,11 @@
           <t>Công ty TNHH TM DV XD Thuận An Phát</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>107.145429,10.396603,0</t>
-        </is>
+      <c r="B75" t="n">
+        <v>107.145429</v>
+      </c>
+      <c r="C75" t="n">
+        <v>10.396603</v>
       </c>
     </row>
     <row r="76">
@@ -1339,10 +1418,11 @@
           <t>Cửa Hàng Máy Móc - Thiết Bị Xây Dựng Bá Tuấn</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>107.054428,10.601561,0</t>
-        </is>
+      <c r="B76" t="n">
+        <v>107.054428</v>
+      </c>
+      <c r="C76" t="n">
+        <v>10.601561</v>
       </c>
     </row>
     <row r="77">
@@ -1351,10 +1431,11 @@
           <t>Cửa Hàng Vlxd Thăng Long</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>107.053976,10.582563,0</t>
-        </is>
+      <c r="B77" t="n">
+        <v>107.053976</v>
+      </c>
+      <c r="C77" t="n">
+        <v>10.582563</v>
       </c>
     </row>
     <row r="78">
@@ -1363,10 +1444,11 @@
           <t>Cửa Hàng Vlxd Minh Nhật</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>107.056196,10.573441,0</t>
-        </is>
+      <c r="B78" t="n">
+        <v>107.056196</v>
+      </c>
+      <c r="C78" t="n">
+        <v>10.573441</v>
       </c>
     </row>
     <row r="79">
@@ -1375,10 +1457,11 @@
           <t>Cửa Hàng Vlxd Đức Cửu</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>107.073281,10.539833,0</t>
-        </is>
+      <c r="B79" t="n">
+        <v>107.073281</v>
+      </c>
+      <c r="C79" t="n">
+        <v>10.539833</v>
       </c>
     </row>
     <row r="80">
@@ -1387,10 +1470,11 @@
           <t>Cửa Hàng Vlxd Năm Mầm</t>
         </is>
       </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>107.086087,10.517281,0</t>
-        </is>
+      <c r="B80" t="n">
+        <v>107.086087</v>
+      </c>
+      <c r="C80" t="n">
+        <v>10.517281</v>
       </c>
     </row>
     <row r="81">
@@ -1399,10 +1483,11 @@
           <t>Cửa Hàng Vlxd Thành Chí</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>107.169335,10.475711,0</t>
-        </is>
+      <c r="B81" t="n">
+        <v>107.169335</v>
+      </c>
+      <c r="C81" t="n">
+        <v>10.475711</v>
       </c>
     </row>
     <row r="82">
@@ -1411,10 +1496,11 @@
           <t>CÔNG TY TNHH VLXD MINH THÀNH ĐẠT</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>107.151217,10.500832,0</t>
-        </is>
+      <c r="B82" t="n">
+        <v>107.151217</v>
+      </c>
+      <c r="C82" t="n">
+        <v>10.500832</v>
       </c>
     </row>
     <row r="83">
@@ -1423,10 +1509,11 @@
           <t>Cửa Hàng Vlxd Hải Sơn</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>107.076038,10.533997,0</t>
-        </is>
+      <c r="B83" t="n">
+        <v>107.076038</v>
+      </c>
+      <c r="C83" t="n">
+        <v>10.533997</v>
       </c>
     </row>
     <row r="84">
@@ -1435,10 +1522,11 @@
           <t>Cửa Hàng Ống Nhựa Bình Minh Hà Dương</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>107.090898,10.521031,0</t>
-        </is>
+      <c r="B84" t="n">
+        <v>107.090898</v>
+      </c>
+      <c r="C84" t="n">
+        <v>10.521031</v>
       </c>
     </row>
     <row r="85">
@@ -1447,10 +1535,11 @@
           <t>Cửa hàng điện nước minh phát 2</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>107.07074,10.588992,0</t>
-        </is>
+      <c r="B85" t="n">
+        <v>107.07074</v>
+      </c>
+      <c r="C85" t="n">
+        <v>10.588992</v>
       </c>
     </row>
     <row r="86">
@@ -1459,10 +1548,11 @@
           <t>KNG MALL PHÚ MỸ</t>
         </is>
       </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>107.056148,10.588926,0</t>
-        </is>
+      <c r="B86" t="n">
+        <v>107.056148</v>
+      </c>
+      <c r="C86" t="n">
+        <v>10.588926</v>
       </c>
     </row>
     <row r="87">
@@ -1471,10 +1561,11 @@
           <t>Cửa hàng vật liệu xây dựng Quốc Thắng</t>
         </is>
       </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>107.0674,10.587771,0</t>
-        </is>
+      <c r="B87" t="n">
+        <v>107.0674</v>
+      </c>
+      <c r="C87" t="n">
+        <v>10.587771</v>
       </c>
     </row>
     <row r="88">
@@ -1483,10 +1574,11 @@
           <t>Cửa Hàng Vlxd Lý Lương</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>107.068026,10.596736,0</t>
-        </is>
+      <c r="B88" t="n">
+        <v>107.068026</v>
+      </c>
+      <c r="C88" t="n">
+        <v>10.596736</v>
       </c>
     </row>
     <row r="89">
@@ -1495,10 +1587,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Tuyết Hồng</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>107.055012,10.597199,0</t>
-        </is>
+      <c r="B89" t="n">
+        <v>107.055012</v>
+      </c>
+      <c r="C89" t="n">
+        <v>10.597199</v>
       </c>
     </row>
     <row r="90">
@@ -1507,10 +1600,11 @@
           <t>Công Ty Tnhh Vlxd Kiên Long</t>
         </is>
       </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>107.18898,10.509704,0</t>
-        </is>
+      <c r="B90" t="n">
+        <v>107.18898</v>
+      </c>
+      <c r="C90" t="n">
+        <v>10.509704</v>
       </c>
     </row>
     <row r="91">
@@ -1519,10 +1613,11 @@
           <t>Cửa Hàng Vlxd Đức Thông</t>
         </is>
       </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>107.19685,10.528083,0</t>
-        </is>
+      <c r="B91" t="n">
+        <v>107.19685</v>
+      </c>
+      <c r="C91" t="n">
+        <v>10.528083</v>
       </c>
     </row>
     <row r="92">
@@ -1531,10 +1626,11 @@
           <t>Cửa Hàng Vlxd &amp; Trang Trí Nội Thất Đức Dũng</t>
         </is>
       </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>107.245432,10.698705,0</t>
-        </is>
+      <c r="B92" t="n">
+        <v>107.245432</v>
+      </c>
+      <c r="C92" t="n">
+        <v>10.698705</v>
       </c>
     </row>
     <row r="93">
@@ -1543,10 +1639,11 @@
           <t>Cửa Hàng Vlxd &amp; Trang Trí Nội Thất Trí Đức</t>
         </is>
       </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>107.247852,10.677785,0</t>
-        </is>
+      <c r="B93" t="n">
+        <v>107.247852</v>
+      </c>
+      <c r="C93" t="n">
+        <v>10.677785</v>
       </c>
     </row>
     <row r="94">
@@ -1555,10 +1652,11 @@
           <t>Tôn Hoa Sen - Cửa Hàng Châu đức</t>
         </is>
       </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>107.248377,10.672644,0</t>
-        </is>
+      <c r="B94" t="n">
+        <v>107.248377</v>
+      </c>
+      <c r="C94" t="n">
+        <v>10.672644</v>
       </c>
     </row>
     <row r="95">
@@ -1567,10 +1665,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Khánh Miên</t>
         </is>
       </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>107.244858,10.641306,0</t>
-        </is>
+      <c r="B95" t="n">
+        <v>107.244858</v>
+      </c>
+      <c r="C95" t="n">
+        <v>10.641306</v>
       </c>
     </row>
     <row r="96">
@@ -1579,10 +1678,11 @@
           <t>Cửa Hàng Vlxd - Trang Trí Nội Thất Đức Linh</t>
         </is>
       </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>107.263289,10.649786,0</t>
-        </is>
+      <c r="B96" t="n">
+        <v>107.263289</v>
+      </c>
+      <c r="C96" t="n">
+        <v>10.649786</v>
       </c>
     </row>
     <row r="97">
@@ -1591,10 +1691,11 @@
           <t>Showroom VLXD - TTNT Quang - Bảy Thép</t>
         </is>
       </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>107.245854,10.64791,0</t>
-        </is>
+      <c r="B97" t="n">
+        <v>107.245854</v>
+      </c>
+      <c r="C97" t="n">
+        <v>10.64791</v>
       </c>
     </row>
     <row r="98">
@@ -1603,10 +1704,11 @@
           <t>Cửa Hàng Vlxd Vinh Tiến</t>
         </is>
       </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>107.316078,10.64359,0</t>
-        </is>
+      <c r="B98" t="n">
+        <v>107.316078</v>
+      </c>
+      <c r="C98" t="n">
+        <v>10.64359</v>
       </c>
     </row>
     <row r="99">
@@ -1615,10 +1717,11 @@
           <t>Cửa Hàng Vlxd Duy Trí</t>
         </is>
       </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>107.242603,10.635497,0</t>
-        </is>
+      <c r="B99" t="n">
+        <v>107.242603</v>
+      </c>
+      <c r="C99" t="n">
+        <v>10.635497</v>
       </c>
     </row>
     <row r="100">
@@ -1627,10 +1730,11 @@
           <t>Mai Sơn Co. Ltd</t>
         </is>
       </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>107.245182,10.644182,0</t>
-        </is>
+      <c r="B100" t="n">
+        <v>107.245182</v>
+      </c>
+      <c r="C100" t="n">
+        <v>10.644182</v>
       </c>
     </row>
     <row r="101">
@@ -1639,10 +1743,11 @@
           <t>Cửa Hàng Vlxd Việt Trung</t>
         </is>
       </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>107.248338,10.660792,0</t>
-        </is>
+      <c r="B101" t="n">
+        <v>107.248338</v>
+      </c>
+      <c r="C101" t="n">
+        <v>10.660792</v>
       </c>
     </row>
     <row r="102">
@@ -1651,10 +1756,11 @@
           <t>Cửa hàng VLXD Chín lác</t>
         </is>
       </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>107.232978,10.64943,0</t>
-        </is>
+      <c r="B102" t="n">
+        <v>107.232978</v>
+      </c>
+      <c r="C102" t="n">
+        <v>10.64943</v>
       </c>
     </row>
     <row r="103">
@@ -1663,10 +1769,11 @@
           <t>VlXD DŨNG HUẾ</t>
         </is>
       </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>107.240391,10.703826,0</t>
-        </is>
+      <c r="B103" t="n">
+        <v>107.240391</v>
+      </c>
+      <c r="C103" t="n">
+        <v>10.703826</v>
       </c>
     </row>
     <row r="104">
@@ -1675,10 +1782,11 @@
           <t>Cửa hàng VLXD Trí Tài</t>
         </is>
       </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>107.241907,10.711214,0</t>
-        </is>
+      <c r="B104" t="n">
+        <v>107.241907</v>
+      </c>
+      <c r="C104" t="n">
+        <v>10.711214</v>
       </c>
     </row>
     <row r="105">
@@ -1687,10 +1795,11 @@
           <t>Cửa Hàng Vlxd Ngọc</t>
         </is>
       </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>107.239412,10.724138,0</t>
-        </is>
+      <c r="B105" t="n">
+        <v>107.239412</v>
+      </c>
+      <c r="C105" t="n">
+        <v>10.724138</v>
       </c>
     </row>
     <row r="106">
@@ -1699,10 +1808,11 @@
           <t>Vật Liệu Xây Dựng Thanh Hoà</t>
         </is>
       </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>107.154627,10.579786,0</t>
-        </is>
+      <c r="B106" t="n">
+        <v>107.154627</v>
+      </c>
+      <c r="C106" t="n">
+        <v>10.579786</v>
       </c>
     </row>
     <row r="107">
@@ -1711,10 +1821,11 @@
           <t>Doanh Nghiệp Tư Nhân Xuân Thúy</t>
         </is>
       </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>107.147047,10.588457,0</t>
-        </is>
+      <c r="B107" t="n">
+        <v>107.147047</v>
+      </c>
+      <c r="C107" t="n">
+        <v>10.588457</v>
       </c>
     </row>
     <row r="108">
@@ -1723,10 +1834,11 @@
           <t>Công ty TNHH vật liệu xây dựng Thanh Nhung</t>
         </is>
       </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>107.13305,10.590313,0</t>
-        </is>
+      <c r="B108" t="n">
+        <v>107.13305</v>
+      </c>
+      <c r="C108" t="n">
+        <v>10.590313</v>
       </c>
     </row>
     <row r="109">
@@ -1735,10 +1847,11 @@
           <t>Cty TNHH VLXD Long Tân</t>
         </is>
       </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>107.125005,10.37804,0</t>
-        </is>
+      <c r="B109" t="n">
+        <v>107.125005</v>
+      </c>
+      <c r="C109" t="n">
+        <v>10.37804</v>
       </c>
     </row>
     <row r="110">
@@ -1747,10 +1860,11 @@
           <t>Cửa Hàng Vlxd Bá Tấn</t>
         </is>
       </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>107.191169,10.407923,0</t>
-        </is>
+      <c r="B110" t="n">
+        <v>107.191169</v>
+      </c>
+      <c r="C110" t="n">
+        <v>10.407923</v>
       </c>
     </row>
     <row r="111">
@@ -1759,10 +1873,11 @@
           <t>Cửa Hàng Vlxd Tân Thịnh Phát</t>
         </is>
       </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>107.121047,10.40112,0</t>
-        </is>
+      <c r="B111" t="n">
+        <v>107.121047</v>
+      </c>
+      <c r="C111" t="n">
+        <v>10.40112</v>
       </c>
     </row>
     <row r="112">
@@ -1771,10 +1886,11 @@
           <t>CỬA HÀNG VLXD THÀNH ĐẠT</t>
         </is>
       </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>107.092875,10.46457,0</t>
-        </is>
+      <c r="B112" t="n">
+        <v>107.092875</v>
+      </c>
+      <c r="C112" t="n">
+        <v>10.46457</v>
       </c>
     </row>
     <row r="113">
@@ -1783,10 +1899,11 @@
           <t>Cửa Hàng VLXD Thanh Bạch</t>
         </is>
       </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>107.076429,10.461287,0</t>
-        </is>
+      <c r="B113" t="n">
+        <v>107.076429</v>
+      </c>
+      <c r="C113" t="n">
+        <v>10.461287</v>
       </c>
     </row>
     <row r="114">
@@ -1795,10 +1912,11 @@
           <t>Cửa Hàng Vlxd Hồng Phúc</t>
         </is>
       </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>107.218464,10.415371,0</t>
-        </is>
+      <c r="B114" t="n">
+        <v>107.218464</v>
+      </c>
+      <c r="C114" t="n">
+        <v>10.415371</v>
       </c>
     </row>
     <row r="115">
@@ -1807,10 +1925,11 @@
           <t>Cửa Hàng Vlxd Quảng Yến</t>
         </is>
       </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>107.211602,10.414037,0</t>
-        </is>
+      <c r="B115" t="n">
+        <v>107.211602</v>
+      </c>
+      <c r="C115" t="n">
+        <v>10.414037</v>
       </c>
     </row>
     <row r="116">
@@ -1819,10 +1938,11 @@
           <t>Công ty TNHH Đầu Tư Thương Mại Xây Dựng Phước An</t>
         </is>
       </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>107.125094,10.40374,0</t>
-        </is>
+      <c r="B116" t="n">
+        <v>107.125094</v>
+      </c>
+      <c r="C116" t="n">
+        <v>10.40374</v>
       </c>
     </row>
     <row r="117">
@@ -1831,10 +1951,11 @@
           <t>Cửa Hàng Vlxd - Trang Trí Nội Thất Đại Lộc</t>
         </is>
       </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>107.39544,10.534072,0</t>
-        </is>
+      <c r="B117" t="n">
+        <v>107.39544</v>
+      </c>
+      <c r="C117" t="n">
+        <v>10.534072</v>
       </c>
     </row>
     <row r="118">
@@ -1843,10 +1964,11 @@
           <t>Cửa Hàng Vlxd Đại Lợi</t>
         </is>
       </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>107.422473,10.543098,0</t>
-        </is>
+      <c r="B118" t="n">
+        <v>107.422473</v>
+      </c>
+      <c r="C118" t="n">
+        <v>10.543098</v>
       </c>
     </row>
     <row r="119">
@@ -1855,10 +1977,11 @@
           <t>Cửa Hàng Vlxd Thành Lợi</t>
         </is>
       </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>107.546378,10.556951,0</t>
-        </is>
+      <c r="B119" t="n">
+        <v>107.546378</v>
+      </c>
+      <c r="C119" t="n">
+        <v>10.556951</v>
       </c>
     </row>
     <row r="120">
@@ -1867,10 +1990,11 @@
           <t>VLXD Lâm Thủy</t>
         </is>
       </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>107.423355,10.565545,0</t>
-        </is>
+      <c r="B120" t="n">
+        <v>107.423355</v>
+      </c>
+      <c r="C120" t="n">
+        <v>10.565545</v>
       </c>
     </row>
     <row r="121">
@@ -1879,10 +2003,11 @@
           <t>CỬA HÀNG VẬT LIỆU XÂY DỰNG THIÊN PHÚC</t>
         </is>
       </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>107.552778,10.579325,0</t>
-        </is>
+      <c r="B121" t="n">
+        <v>107.552778</v>
+      </c>
+      <c r="C121" t="n">
+        <v>10.579325</v>
       </c>
     </row>
     <row r="122">
@@ -1891,10 +2016,11 @@
           <t>Cửa Hàng Vlxd Hai Thu</t>
         </is>
       </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>107.558711,10.582886,0</t>
-        </is>
+      <c r="B122" t="n">
+        <v>107.558711</v>
+      </c>
+      <c r="C122" t="n">
+        <v>10.582886</v>
       </c>
     </row>
     <row r="123">
@@ -1903,10 +2029,11 @@
           <t>VLXD Thanh Hải</t>
         </is>
       </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>107.3818,10.656973,0</t>
-        </is>
+      <c r="B123" t="n">
+        <v>107.3818</v>
+      </c>
+      <c r="C123" t="n">
+        <v>10.656973</v>
       </c>
     </row>
     <row r="124">
@@ -1915,10 +2042,11 @@
           <t>Cửa Hàng Vlxd Năm Khuyến</t>
         </is>
       </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>107.387867,10.682568,0</t>
-        </is>
+      <c r="B124" t="n">
+        <v>107.387867</v>
+      </c>
+      <c r="C124" t="n">
+        <v>10.682568</v>
       </c>
     </row>
     <row r="125">
@@ -1927,10 +2055,11 @@
           <t>Cửa Hàng Vlxd Minh Chiến</t>
         </is>
       </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>107.501156,10.68958,0</t>
-        </is>
+      <c r="B125" t="n">
+        <v>107.501156</v>
+      </c>
+      <c r="C125" t="n">
+        <v>10.68958</v>
       </c>
     </row>
     <row r="126">
@@ -1939,10 +2068,11 @@
           <t>Cửa Hàng Vlxd Phan Văn Thành</t>
         </is>
       </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>107.407058,10.728223,0</t>
-        </is>
+      <c r="B126" t="n">
+        <v>107.407058</v>
+      </c>
+      <c r="C126" t="n">
+        <v>10.728223</v>
       </c>
     </row>
     <row r="127">
@@ -1951,10 +2081,11 @@
           <t>Vật Liệu Xây Dựng Tân Tiến</t>
         </is>
       </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>107.06076,10.562716,0</t>
-        </is>
+      <c r="B127" t="n">
+        <v>107.06076</v>
+      </c>
+      <c r="C127" t="n">
+        <v>10.562716</v>
       </c>
     </row>
     <row r="128">
@@ -1963,10 +2094,11 @@
           <t>Cửa hàng VLXD Thạch Loan</t>
         </is>
       </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>107.071032,10.546983,0</t>
-        </is>
+      <c r="B128" t="n">
+        <v>107.071032</v>
+      </c>
+      <c r="C128" t="n">
+        <v>10.546983</v>
       </c>
     </row>
     <row r="129">
@@ -1975,10 +2107,11 @@
           <t>Cửa Hàng Vlxd Văn Thắng</t>
         </is>
       </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>107.048562,10.632887,0</t>
-        </is>
+      <c r="B129" t="n">
+        <v>107.048562</v>
+      </c>
+      <c r="C129" t="n">
+        <v>10.632887</v>
       </c>
     </row>
     <row r="130">
@@ -1987,10 +2120,11 @@
           <t>Cửa Hàng VLXD Thanh Tùng</t>
         </is>
       </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>107.054874,10.604932,0</t>
-        </is>
+      <c r="B130" t="n">
+        <v>107.054874</v>
+      </c>
+      <c r="C130" t="n">
+        <v>10.604932</v>
       </c>
     </row>
     <row r="131">
@@ -1999,10 +2133,11 @@
           <t>Cửa Hàng Vlxd Vinh</t>
         </is>
       </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>107.059569,10.586266,0</t>
-        </is>
+      <c r="B131" t="n">
+        <v>107.059569</v>
+      </c>
+      <c r="C131" t="n">
+        <v>10.586266</v>
       </c>
     </row>
     <row r="132">
@@ -2011,10 +2146,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Đức Khang</t>
         </is>
       </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>107.126348,10.643938,0</t>
-        </is>
+      <c r="B132" t="n">
+        <v>107.126348</v>
+      </c>
+      <c r="C132" t="n">
+        <v>10.643938</v>
       </c>
     </row>
     <row r="133">
@@ -2023,10 +2159,11 @@
           <t>Cửa Hàng Vlxd Hoàng Nam</t>
         </is>
       </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>107.056419,10.624509,0</t>
-        </is>
+      <c r="B133" t="n">
+        <v>107.056419</v>
+      </c>
+      <c r="C133" t="n">
+        <v>10.624509</v>
       </c>
     </row>
     <row r="134">
@@ -2035,10 +2172,11 @@
           <t>VLXD Luong Tung</t>
         </is>
       </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>107.0925,10.641055,0</t>
-        </is>
+      <c r="B134" t="n">
+        <v>107.0925</v>
+      </c>
+      <c r="C134" t="n">
+        <v>10.641055</v>
       </c>
     </row>
     <row r="135">
@@ -2047,10 +2185,11 @@
           <t>Vật Liệu Xây Dựng Thành Luân</t>
         </is>
       </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>107.069679,10.630513,0</t>
-        </is>
+      <c r="B135" t="n">
+        <v>107.069679</v>
+      </c>
+      <c r="C135" t="n">
+        <v>10.630513</v>
       </c>
     </row>
     <row r="136">
@@ -2059,10 +2198,11 @@
           <t>Cửa Hàng Gạch Men Phong Phát</t>
         </is>
       </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>107.104628,10.643718,0</t>
-        </is>
+      <c r="B136" t="n">
+        <v>107.104628</v>
+      </c>
+      <c r="C136" t="n">
+        <v>10.643718</v>
       </c>
     </row>
     <row r="137">
@@ -2071,10 +2211,11 @@
           <t>VLXD Anh Tường</t>
         </is>
       </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>107.084629,10.639186,0</t>
-        </is>
+      <c r="B137" t="n">
+        <v>107.084629</v>
+      </c>
+      <c r="C137" t="n">
+        <v>10.639186</v>
       </c>
     </row>
     <row r="138">
@@ -2083,10 +2224,11 @@
           <t>VLXD Chúng Và</t>
         </is>
       </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>107.161884,10.656524,0</t>
-        </is>
+      <c r="B138" t="n">
+        <v>107.161884</v>
+      </c>
+      <c r="C138" t="n">
+        <v>10.656524</v>
       </c>
     </row>
     <row r="139">
@@ -2095,10 +2237,11 @@
           <t>VLXD Nguyên Linh</t>
         </is>
       </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>107.168339,10.654357,0</t>
-        </is>
+      <c r="B139" t="n">
+        <v>107.168339</v>
+      </c>
+      <c r="C139" t="n">
+        <v>10.654357</v>
       </c>
     </row>
     <row r="140">
@@ -2107,10 +2250,11 @@
           <t>Cửa hàng VLXD Nhật Huy</t>
         </is>
       </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>107.331577,10.456957,0</t>
-        </is>
+      <c r="B140" t="n">
+        <v>107.331577</v>
+      </c>
+      <c r="C140" t="n">
+        <v>10.456957</v>
       </c>
     </row>
     <row r="141">
@@ -2119,10 +2263,11 @@
           <t>Cửa hàng VLXD Hải Vân</t>
         </is>
       </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>107.41903,10.567846,0</t>
-        </is>
+      <c r="B141" t="n">
+        <v>107.41903</v>
+      </c>
+      <c r="C141" t="n">
+        <v>10.567846</v>
       </c>
     </row>
     <row r="142">
@@ -2131,10 +2276,11 @@
           <t>Cửa hàng VLXD Đại Lộc Phát</t>
         </is>
       </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>107.386347,10.529842,0</t>
-        </is>
+      <c r="B142" t="n">
+        <v>107.386347</v>
+      </c>
+      <c r="C142" t="n">
+        <v>10.529842</v>
       </c>
     </row>
     <row r="143">
@@ -2143,10 +2289,11 @@
           <t>Cửa Hàng Vlxd Chấn Long</t>
         </is>
       </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>107.214473,10.48478,0</t>
-        </is>
+      <c r="B143" t="n">
+        <v>107.214473</v>
+      </c>
+      <c r="C143" t="n">
+        <v>10.48478</v>
       </c>
     </row>
     <row r="144">
@@ -2155,10 +2302,11 @@
           <t>Công Ty TNHH Vật Liệu Xây Dựng Long Tân</t>
         </is>
       </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>107.210438,10.481312,0</t>
-        </is>
+      <c r="B144" t="n">
+        <v>107.210438</v>
+      </c>
+      <c r="C144" t="n">
+        <v>10.481312</v>
       </c>
     </row>
     <row r="145">
@@ -2167,10 +2315,11 @@
           <t>Cửa Hàng VLXD Hải Vân</t>
         </is>
       </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>107.213807,10.486449,0</t>
-        </is>
+      <c r="B145" t="n">
+        <v>107.213807</v>
+      </c>
+      <c r="C145" t="n">
+        <v>10.486449</v>
       </c>
     </row>
     <row r="146">
@@ -2179,10 +2328,11 @@
           <t>Cửa Hàng Vlxd Hoàng Dũng</t>
         </is>
       </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>107.200051,10.498538,0</t>
-        </is>
+      <c r="B146" t="n">
+        <v>107.200051</v>
+      </c>
+      <c r="C146" t="n">
+        <v>10.498538</v>
       </c>
     </row>
     <row r="147">
@@ -2191,10 +2341,11 @@
           <t>VLXD Xuân Hòa</t>
         </is>
       </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>107.388781,10.552796,0</t>
-        </is>
+      <c r="B147" t="n">
+        <v>107.388781</v>
+      </c>
+      <c r="C147" t="n">
+        <v>10.552796</v>
       </c>
     </row>
     <row r="148">
@@ -2203,10 +2354,11 @@
           <t>Cửa Hàng Vlxd Xuân Ngọc</t>
         </is>
       </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>107.439096,10.609973,0</t>
-        </is>
+      <c r="B148" t="n">
+        <v>107.439096</v>
+      </c>
+      <c r="C148" t="n">
+        <v>10.609973</v>
       </c>
     </row>
     <row r="149">
@@ -2215,10 +2367,11 @@
           <t>Cửa Hàng Vlxd Thảo Nam</t>
         </is>
       </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>107.374028,10.637221,0</t>
-        </is>
+      <c r="B149" t="n">
+        <v>107.374028</v>
+      </c>
+      <c r="C149" t="n">
+        <v>10.637221</v>
       </c>
     </row>
     <row r="150">
@@ -2227,10 +2380,11 @@
           <t>Cửa Hàng Vlxd Tân Phát</t>
         </is>
       </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>107.449114,10.629166,0</t>
-        </is>
+      <c r="B150" t="n">
+        <v>107.449114</v>
+      </c>
+      <c r="C150" t="n">
+        <v>10.629166</v>
       </c>
     </row>
     <row r="151">
@@ -2239,10 +2393,11 @@
           <t>VLXD ĐẠI HUỲNH</t>
         </is>
       </c>
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>107.449656,10.630084,0</t>
-        </is>
+      <c r="B151" t="n">
+        <v>107.449656</v>
+      </c>
+      <c r="C151" t="n">
+        <v>10.630084</v>
       </c>
     </row>
     <row r="152">
@@ -2251,10 +2406,11 @@
           <t>Cửa Hàng Vlxd Vân Vũ</t>
         </is>
       </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>107.294546,10.42679,0</t>
-        </is>
+      <c r="B152" t="n">
+        <v>107.294546</v>
+      </c>
+      <c r="C152" t="n">
+        <v>10.42679</v>
       </c>
     </row>
     <row r="153">
@@ -2263,10 +2419,11 @@
           <t>Cửa Hàng Vlxd Hữu Tài</t>
         </is>
       </c>
-      <c r="B153" t="inlineStr">
-        <is>
-          <t>107.293063,10.429522,0</t>
-        </is>
+      <c r="B153" t="n">
+        <v>107.293063</v>
+      </c>
+      <c r="C153" t="n">
+        <v>10.429522</v>
       </c>
     </row>
     <row r="154">
@@ -2275,10 +2432,11 @@
           <t>Cửa Hàng Vlxd Phương Quang</t>
         </is>
       </c>
-      <c r="B154" t="inlineStr">
-        <is>
-          <t>107.329007,10.455819,0</t>
-        </is>
+      <c r="B154" t="n">
+        <v>107.329007</v>
+      </c>
+      <c r="C154" t="n">
+        <v>10.455819</v>
       </c>
     </row>
     <row r="155">
@@ -2287,10 +2445,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Hạnh</t>
         </is>
       </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>107.285747,10.444187,0</t>
-        </is>
+      <c r="B155" t="n">
+        <v>107.285747</v>
+      </c>
+      <c r="C155" t="n">
+        <v>10.444187</v>
       </c>
     </row>
     <row r="156">
@@ -2299,10 +2458,11 @@
           <t>Kho VLXD Mai Hưng Thịnh</t>
         </is>
       </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>107.311676,10.489486,0</t>
-        </is>
+      <c r="B156" t="n">
+        <v>107.311676</v>
+      </c>
+      <c r="C156" t="n">
+        <v>10.489486</v>
       </c>
     </row>
     <row r="157">
@@ -2311,10 +2471,11 @@
           <t>Vật Liệu Xây Dựng - Thiết Bị Vệ Sinh , Bếp Cao Cấp Kim Dũng</t>
         </is>
       </c>
-      <c r="B157" t="inlineStr">
-        <is>
-          <t>107.297188,10.500812,0</t>
-        </is>
+      <c r="B157" t="n">
+        <v>107.297188</v>
+      </c>
+      <c r="C157" t="n">
+        <v>10.500812</v>
       </c>
     </row>
     <row r="158">
@@ -2323,10 +2484,11 @@
           <t>Cửa Hàng Tôn Sắt Phương Thành</t>
         </is>
       </c>
-      <c r="B158" t="inlineStr">
-        <is>
-          <t>107.214403,10.540293,0</t>
-        </is>
+      <c r="B158" t="n">
+        <v>107.214403</v>
+      </c>
+      <c r="C158" t="n">
+        <v>10.540293</v>
       </c>
     </row>
     <row r="159">
@@ -2335,10 +2497,11 @@
           <t>KHANH - Cửa hàng Máy và Dụng cụ Xây Dựng Bà Rịa , Vũng Tàu</t>
         </is>
       </c>
-      <c r="B159" t="inlineStr">
-        <is>
-          <t>107.383256,10.55831,0</t>
-        </is>
+      <c r="B159" t="n">
+        <v>107.383256</v>
+      </c>
+      <c r="C159" t="n">
+        <v>10.55831</v>
       </c>
     </row>
     <row r="160">
@@ -2347,10 +2510,11 @@
           <t>Cửa Hàng Vlxd Tân Phước Thuận</t>
         </is>
       </c>
-      <c r="B160" t="inlineStr">
-        <is>
-          <t>107.43167,10.558723,0</t>
-        </is>
+      <c r="B160" t="n">
+        <v>107.43167</v>
+      </c>
+      <c r="C160" t="n">
+        <v>10.558723</v>
       </c>
     </row>
     <row r="161">
@@ -2359,10 +2523,11 @@
           <t>Kỹ Nghệ Sắt Vĩnh Bình</t>
         </is>
       </c>
-      <c r="B161" t="inlineStr">
-        <is>
-          <t>107.391776,10.548099,0</t>
-        </is>
+      <c r="B161" t="n">
+        <v>107.391776</v>
+      </c>
+      <c r="C161" t="n">
+        <v>10.548099</v>
       </c>
     </row>
     <row r="162">
@@ -2371,10 +2536,11 @@
           <t>Cửa Hàng Trần La Phông Hoàng Phương 4</t>
         </is>
       </c>
-      <c r="B162" t="inlineStr">
-        <is>
-          <t>107.389549,10.531233,0</t>
-        </is>
+      <c r="B162" t="n">
+        <v>107.389549</v>
+      </c>
+      <c r="C162" t="n">
+        <v>10.531233</v>
       </c>
     </row>
     <row r="163">
@@ -2383,10 +2549,11 @@
           <t>Cửa Hàng Vlxd Vân Truyền</t>
         </is>
       </c>
-      <c r="B163" t="inlineStr">
-        <is>
-          <t>107.277804,10.461339,0</t>
-        </is>
+      <c r="B163" t="n">
+        <v>107.277804</v>
+      </c>
+      <c r="C163" t="n">
+        <v>10.461339</v>
       </c>
     </row>
     <row r="164">
@@ -2395,10 +2562,11 @@
           <t>Cửa hàng Vật Liệu Xây Dựng Hải Trang</t>
         </is>
       </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>107.090481,10.515927,0</t>
-        </is>
+      <c r="B164" t="n">
+        <v>107.090481</v>
+      </c>
+      <c r="C164" t="n">
+        <v>10.515927</v>
       </c>
     </row>
     <row r="165">
@@ -2407,10 +2575,11 @@
           <t>Hoàng Trọng Cửa Hàng Kinh Doanh Sắt Thép,Sắt Xây Dựng</t>
         </is>
       </c>
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>107.090069,10.520942,0</t>
-        </is>
+      <c r="B165" t="n">
+        <v>107.090069</v>
+      </c>
+      <c r="C165" t="n">
+        <v>10.520942</v>
       </c>
     </row>
     <row r="166">
@@ -2419,10 +2588,11 @@
           <t>Sắt Thép SEN VIỆT (Minh Khuê cũ)</t>
         </is>
       </c>
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>107.078086,10.532786,0</t>
-        </is>
+      <c r="B166" t="n">
+        <v>107.078086</v>
+      </c>
+      <c r="C166" t="n">
+        <v>10.532786</v>
       </c>
     </row>
     <row r="167">
@@ -2431,10 +2601,11 @@
           <t>Cửa Hàng Vlxd Đô Lương</t>
         </is>
       </c>
-      <c r="B167" t="inlineStr">
-        <is>
-          <t>107.144151,10.403205,0</t>
-        </is>
+      <c r="B167" t="n">
+        <v>107.144151</v>
+      </c>
+      <c r="C167" t="n">
+        <v>10.403205</v>
       </c>
     </row>
     <row r="168">
@@ -2443,10 +2614,11 @@
           <t>Của Hàng Vlxd Mai Chi</t>
         </is>
       </c>
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>107.170701,10.532021,0</t>
-        </is>
+      <c r="B168" t="n">
+        <v>107.170701</v>
+      </c>
+      <c r="C168" t="n">
+        <v>10.532021</v>
       </c>
     </row>
     <row r="169">
@@ -2455,10 +2627,11 @@
           <t>Đại lý PP bếp điện từ CIVIN - Vlxd Cúc Nguyễn</t>
         </is>
       </c>
-      <c r="B169" t="inlineStr">
-        <is>
-          <t>107.183366,10.677129,0</t>
-        </is>
+      <c r="B169" t="n">
+        <v>107.183366</v>
+      </c>
+      <c r="C169" t="n">
+        <v>10.677129</v>
       </c>
     </row>
     <row r="170">
@@ -2467,10 +2640,11 @@
           <t>Cửa Hàng VLXD Minh Trâm</t>
         </is>
       </c>
-      <c r="B170" t="inlineStr">
-        <is>
-          <t>107.398371,10.526114,0</t>
-        </is>
+      <c r="B170" t="n">
+        <v>107.398371</v>
+      </c>
+      <c r="C170" t="n">
+        <v>10.526114</v>
       </c>
     </row>
     <row r="171">
@@ -2479,10 +2653,11 @@
           <t>Vật Liệu Xây Dựng - Kho Gạch Men PHƯƠNG LINH</t>
         </is>
       </c>
-      <c r="B171" t="inlineStr">
-        <is>
-          <t>107.322347,10.452745,0</t>
-        </is>
+      <c r="B171" t="n">
+        <v>107.322347</v>
+      </c>
+      <c r="C171" t="n">
+        <v>10.452745</v>
       </c>
     </row>
     <row r="172">
@@ -2491,10 +2666,11 @@
           <t>Cửa hàng kd vật tư ttnt &amp; nt Bảo An</t>
         </is>
       </c>
-      <c r="B172" t="inlineStr">
-        <is>
-          <t>107.295584,10.444875,0</t>
-        </is>
+      <c r="B172" t="n">
+        <v>107.295584</v>
+      </c>
+      <c r="C172" t="n">
+        <v>10.444875</v>
       </c>
     </row>
     <row r="173">
@@ -2503,10 +2679,11 @@
           <t>Cửa Hàng Vlxd Kim Ngân</t>
         </is>
       </c>
-      <c r="B173" t="inlineStr">
-        <is>
-          <t>107.347288,10.51428,0</t>
-        </is>
+      <c r="B173" t="n">
+        <v>107.347288</v>
+      </c>
+      <c r="C173" t="n">
+        <v>10.51428</v>
       </c>
     </row>
     <row r="174">
@@ -2515,10 +2692,11 @@
           <t>Cửa Hàng Thiết Bị Xd Minh Nhật</t>
         </is>
       </c>
-      <c r="B174" t="inlineStr">
-        <is>
-          <t>107.429822,10.478572,0</t>
-        </is>
+      <c r="B174" t="n">
+        <v>107.429822</v>
+      </c>
+      <c r="C174" t="n">
+        <v>10.478572</v>
       </c>
     </row>
     <row r="175">
@@ -2527,10 +2705,11 @@
           <t>Đại Lý Ống Nhựa Quốc Minh</t>
         </is>
       </c>
-      <c r="B175" t="inlineStr">
-        <is>
-          <t>107.427089,10.480224,0</t>
-        </is>
+      <c r="B175" t="n">
+        <v>107.427089</v>
+      </c>
+      <c r="C175" t="n">
+        <v>10.480224</v>
       </c>
     </row>
     <row r="176">
@@ -2539,10 +2718,11 @@
           <t>Vật Liệu Xây Dựng HOÀI PHONG</t>
         </is>
       </c>
-      <c r="B176" t="inlineStr">
-        <is>
-          <t>107.271845,10.593688,0</t>
-        </is>
+      <c r="B176" t="n">
+        <v>107.271845</v>
+      </c>
+      <c r="C176" t="n">
+        <v>10.593688</v>
       </c>
     </row>
     <row r="177">
@@ -2551,10 +2731,11 @@
           <t>Vật liệu xây dựng Hùng huy</t>
         </is>
       </c>
-      <c r="B177" t="inlineStr">
-        <is>
-          <t>107.27938,10.594073,0</t>
-        </is>
+      <c r="B177" t="n">
+        <v>107.27938</v>
+      </c>
+      <c r="C177" t="n">
+        <v>10.594073</v>
       </c>
     </row>
     <row r="178">
@@ -2563,10 +2744,11 @@
           <t>BÊ TÔNG THÁI AN</t>
         </is>
       </c>
-      <c r="B178" t="inlineStr">
-        <is>
-          <t>107.295836,10.674773,0</t>
-        </is>
+      <c r="B178" t="n">
+        <v>107.295836</v>
+      </c>
+      <c r="C178" t="n">
+        <v>10.674773</v>
       </c>
     </row>
     <row r="179">
@@ -2575,10 +2757,11 @@
           <t>Cửa Hàng Vlxd Hoàng Hùng</t>
         </is>
       </c>
-      <c r="B179" t="inlineStr">
-        <is>
-          <t>107.315037,10.643172,0</t>
-        </is>
+      <c r="B179" t="n">
+        <v>107.315037</v>
+      </c>
+      <c r="C179" t="n">
+        <v>10.643172</v>
       </c>
     </row>
     <row r="180">
@@ -2587,10 +2770,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Và TRang Trí Nội Thất Châu Phát</t>
         </is>
       </c>
-      <c r="B180" t="inlineStr">
-        <is>
-          <t>107.256987,10.646174,0</t>
-        </is>
+      <c r="B180" t="n">
+        <v>107.256987</v>
+      </c>
+      <c r="C180" t="n">
+        <v>10.646174</v>
       </c>
     </row>
     <row r="181">
@@ -2599,10 +2783,11 @@
           <t>Cửa Hàng Gỗ Xây Dựng Nguyễn Vũ</t>
         </is>
       </c>
-      <c r="B181" t="inlineStr">
-        <is>
-          <t>107.252716,10.644489,0</t>
-        </is>
+      <c r="B181" t="n">
+        <v>107.252716</v>
+      </c>
+      <c r="C181" t="n">
+        <v>10.644489</v>
       </c>
     </row>
     <row r="182">
@@ -2611,10 +2796,11 @@
           <t>Gạch Men Ngọc Hòa</t>
         </is>
       </c>
-      <c r="B182" t="inlineStr">
-        <is>
-          <t>107.253576,10.64427,0</t>
-        </is>
+      <c r="B182" t="n">
+        <v>107.253576</v>
+      </c>
+      <c r="C182" t="n">
+        <v>10.64427</v>
       </c>
     </row>
     <row r="183">
@@ -2623,10 +2809,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Và Hải Sản Bích Ngọc</t>
         </is>
       </c>
-      <c r="B183" t="inlineStr">
-        <is>
-          <t>107.242989,10.645792,0</t>
-        </is>
+      <c r="B183" t="n">
+        <v>107.242989</v>
+      </c>
+      <c r="C183" t="n">
+        <v>10.645792</v>
       </c>
     </row>
     <row r="184">
@@ -2635,10 +2822,11 @@
           <t>Cửa Hàng VLXD THANH</t>
         </is>
       </c>
-      <c r="B184" t="inlineStr">
-        <is>
-          <t>107.327883,10.452854,0</t>
-        </is>
+      <c r="B184" t="n">
+        <v>107.327883</v>
+      </c>
+      <c r="C184" t="n">
+        <v>10.452854</v>
       </c>
     </row>
     <row r="185">
@@ -2647,10 +2835,11 @@
           <t>Cửa Hàng Vlxd Cường Khang</t>
         </is>
       </c>
-      <c r="B185" t="inlineStr">
-        <is>
-          <t>107.327558,10.452954,0</t>
-        </is>
+      <c r="B185" t="n">
+        <v>107.327558</v>
+      </c>
+      <c r="C185" t="n">
+        <v>10.452954</v>
       </c>
     </row>
     <row r="186">
@@ -2659,10 +2848,11 @@
           <t>Showroom Mai Hưng Thịnh</t>
         </is>
       </c>
-      <c r="B186" t="inlineStr">
-        <is>
-          <t>107.327282,10.458759,0</t>
-        </is>
+      <c r="B186" t="n">
+        <v>107.327282</v>
+      </c>
+      <c r="C186" t="n">
+        <v>10.458759</v>
       </c>
     </row>
     <row r="187">
@@ -2671,10 +2861,11 @@
           <t>Cửa Hàng Vlxd Định Hồng</t>
         </is>
       </c>
-      <c r="B187" t="inlineStr">
-        <is>
-          <t>107.448657,10.551997,0</t>
-        </is>
+      <c r="B187" t="n">
+        <v>107.448657</v>
+      </c>
+      <c r="C187" t="n">
+        <v>10.551997</v>
       </c>
     </row>
     <row r="188">
@@ -2683,10 +2874,11 @@
           <t>Cơ Sơ Cửa Sắt Thanh Điền</t>
         </is>
       </c>
-      <c r="B188" t="inlineStr">
-        <is>
-          <t>107.482803,10.552347,0</t>
-        </is>
+      <c r="B188" t="n">
+        <v>107.482803</v>
+      </c>
+      <c r="C188" t="n">
+        <v>10.552347</v>
       </c>
     </row>
     <row r="189">
@@ -2695,10 +2887,11 @@
           <t>Trụ sở chính công ty tnhh nhôm kính Phú vinh</t>
         </is>
       </c>
-      <c r="B189" t="inlineStr">
-        <is>
-          <t>107.487844,10.553423,0</t>
-        </is>
+      <c r="B189" t="n">
+        <v>107.487844</v>
+      </c>
+      <c r="C189" t="n">
+        <v>10.553423</v>
       </c>
     </row>
     <row r="190">
@@ -2707,10 +2900,11 @@
           <t>Cửa Hàng Vlxd Cảnh Nga</t>
         </is>
       </c>
-      <c r="B190" t="inlineStr">
-        <is>
-          <t>107.538724,10.558774,0</t>
-        </is>
+      <c r="B190" t="n">
+        <v>107.538724</v>
+      </c>
+      <c r="C190" t="n">
+        <v>10.558774</v>
       </c>
     </row>
     <row r="191">
@@ -2719,10 +2913,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Tám Trang</t>
         </is>
       </c>
-      <c r="B191" t="inlineStr">
-        <is>
-          <t>107.543628,10.548466,0</t>
-        </is>
+      <c r="B191" t="n">
+        <v>107.543628</v>
+      </c>
+      <c r="C191" t="n">
+        <v>10.548466</v>
       </c>
     </row>
     <row r="192">
@@ -2731,10 +2926,11 @@
           <t>Cửa hàng VLXD MINH TOÀN VŨ</t>
         </is>
       </c>
-      <c r="B192" t="inlineStr">
-        <is>
-          <t>107.491349,10.560251,0</t>
-        </is>
+      <c r="B192" t="n">
+        <v>107.491349</v>
+      </c>
+      <c r="C192" t="n">
+        <v>10.560251</v>
       </c>
     </row>
     <row r="193">
@@ -2743,10 +2939,11 @@
           <t>Cửa hàng VLXD Minh Trâm</t>
         </is>
       </c>
-      <c r="B193" t="inlineStr">
-        <is>
-          <t>107.410959,10.529706,0</t>
-        </is>
+      <c r="B193" t="n">
+        <v>107.410959</v>
+      </c>
+      <c r="C193" t="n">
+        <v>10.529706</v>
       </c>
     </row>
     <row r="194">
@@ -2755,10 +2952,11 @@
           <t>Cửa hàng Nhôm &amp; Thạch Cao 125 Xuyên Mộc</t>
         </is>
       </c>
-      <c r="B194" t="inlineStr">
-        <is>
-          <t>107.419209,10.552676,0</t>
-        </is>
+      <c r="B194" t="n">
+        <v>107.419209</v>
+      </c>
+      <c r="C194" t="n">
+        <v>10.552676</v>
       </c>
     </row>
     <row r="195">
@@ -2767,10 +2965,11 @@
           <t>Cửa hàng VLXD Nội thất Cường Nga</t>
         </is>
       </c>
-      <c r="B195" t="inlineStr">
-        <is>
-          <t>107.118952,10.400278,0</t>
-        </is>
+      <c r="B195" t="n">
+        <v>107.118952</v>
+      </c>
+      <c r="C195" t="n">
+        <v>10.400278</v>
       </c>
     </row>
     <row r="196">
@@ -2779,10 +2978,11 @@
           <t>Cửa Hàng Vlxd Trường Thịnh</t>
         </is>
       </c>
-      <c r="B196" t="inlineStr">
-        <is>
-          <t>107.157088,10.414927,0</t>
-        </is>
+      <c r="B196" t="n">
+        <v>107.157088</v>
+      </c>
+      <c r="C196" t="n">
+        <v>10.414927</v>
       </c>
     </row>
     <row r="197">
@@ -2791,10 +2991,11 @@
           <t>Cửa Hàng Vlxd Trường Phát</t>
         </is>
       </c>
-      <c r="B197" t="inlineStr">
-        <is>
-          <t>107.288178,10.498286,0</t>
-        </is>
+      <c r="B197" t="n">
+        <v>107.288178</v>
+      </c>
+      <c r="C197" t="n">
+        <v>10.498286</v>
       </c>
     </row>
     <row r="198">
@@ -2803,10 +3004,11 @@
           <t>Công Ty Cổ Phần Tư Vấn Xây Dựng Công Nghiệp Phú Mỹ</t>
         </is>
       </c>
-      <c r="B198" t="inlineStr">
-        <is>
-          <t>107.042253,10.595737,0</t>
-        </is>
+      <c r="B198" t="n">
+        <v>107.042253</v>
+      </c>
+      <c r="C198" t="n">
+        <v>10.595737</v>
       </c>
     </row>
     <row r="199">
@@ -2815,10 +3017,11 @@
           <t>Công Ty Tnhh Xây Dựng Và Kd Thương Mại Phú Mỹ</t>
         </is>
       </c>
-      <c r="B199" t="inlineStr">
-        <is>
-          <t>107.053196,10.577114,0</t>
-        </is>
+      <c r="B199" t="n">
+        <v>107.053196</v>
+      </c>
+      <c r="C199" t="n">
+        <v>10.577114</v>
       </c>
     </row>
     <row r="200">
@@ -2827,10 +3030,11 @@
           <t>CTY Xây Dựng Phúc Huy</t>
         </is>
       </c>
-      <c r="B200" t="inlineStr">
-        <is>
-          <t>107.071615,10.625284,0</t>
-        </is>
+      <c r="B200" t="n">
+        <v>107.071615</v>
+      </c>
+      <c r="C200" t="n">
+        <v>10.625284</v>
       </c>
     </row>
     <row r="201">
@@ -2839,10 +3043,11 @@
           <t>Công ty Tư Vấn Thiết Kế Xây Dưng Gạch Block Phú Mỹ</t>
         </is>
       </c>
-      <c r="B201" t="inlineStr">
-        <is>
-          <t>107.07531,10.603212,0</t>
-        </is>
+      <c r="B201" t="n">
+        <v>107.07531</v>
+      </c>
+      <c r="C201" t="n">
+        <v>10.603212</v>
       </c>
     </row>
     <row r="202">
@@ -2851,10 +3056,11 @@
           <t>VLXD Vật Liệu Xây Dựng BẢO BÌNH (chi nhánh 1)</t>
         </is>
       </c>
-      <c r="B202" t="inlineStr">
-        <is>
-          <t>107.2925092,10.8382992,0</t>
-        </is>
+      <c r="B202" t="n">
+        <v>107.2925092</v>
+      </c>
+      <c r="C202" t="n">
+        <v>10.8382992</v>
       </c>
     </row>
     <row r="203">
@@ -2863,10 +3069,11 @@
           <t>Công ty tnhh xây dựng M&amp;E Sao Khuê</t>
         </is>
       </c>
-      <c r="B203" t="inlineStr">
-        <is>
-          <t>107.3562198,10.7928466,0</t>
-        </is>
+      <c r="B203" t="n">
+        <v>107.3562198</v>
+      </c>
+      <c r="C203" t="n">
+        <v>10.7928466</v>
       </c>
     </row>
     <row r="204">
@@ -2875,10 +3082,11 @@
           <t>Dịch vụ sơn sửa nhà Văn Hùng</t>
         </is>
       </c>
-      <c r="B204" t="inlineStr">
-        <is>
-          <t>107.3237412,10.7235384,0</t>
-        </is>
+      <c r="B204" t="n">
+        <v>107.3237412</v>
+      </c>
+      <c r="C204" t="n">
+        <v>10.7235384</v>
       </c>
     </row>
     <row r="205">
@@ -2887,10 +3095,11 @@
           <t>Vật Liệu Xây Dựng Trường Sơn</t>
         </is>
       </c>
-      <c r="B205" t="inlineStr">
-        <is>
-          <t>107.3493865,10.741887,0</t>
-        </is>
+      <c r="B205" t="n">
+        <v>107.3493865</v>
+      </c>
+      <c r="C205" t="n">
+        <v>10.741887</v>
       </c>
     </row>
     <row r="206">
@@ -2899,10 +3108,11 @@
           <t>Quang Phúc Thạch Cao</t>
         </is>
       </c>
-      <c r="B206" t="inlineStr">
-        <is>
-          <t>107.3516031,10.7319087,0</t>
-        </is>
+      <c r="B206" t="n">
+        <v>107.3516031</v>
+      </c>
+      <c r="C206" t="n">
+        <v>10.7319087</v>
       </c>
     </row>
     <row r="207">
@@ -2911,10 +3121,11 @@
           <t>VLXD - HƯNG</t>
         </is>
       </c>
-      <c r="B207" t="inlineStr">
-        <is>
-          <t>107.351576,10.7514674,0</t>
-        </is>
+      <c r="B207" t="n">
+        <v>107.351576</v>
+      </c>
+      <c r="C207" t="n">
+        <v>10.7514674</v>
       </c>
     </row>
     <row r="208">
@@ -2923,10 +3134,11 @@
           <t>VLXD QUANG SƠN</t>
         </is>
       </c>
-      <c r="B208" t="inlineStr">
-        <is>
-          <t>107.351301,10.7475777,0</t>
-        </is>
+      <c r="B208" t="n">
+        <v>107.351301</v>
+      </c>
+      <c r="C208" t="n">
+        <v>10.7475777</v>
       </c>
     </row>
     <row r="209">
@@ -2935,10 +3147,11 @@
           <t>CỬA HÀNG VLXD DIỆU LOAN- Sông Ray</t>
         </is>
       </c>
-      <c r="B209" t="inlineStr">
-        <is>
-          <t>107.3512925,10.7313672,0</t>
-        </is>
+      <c r="B209" t="n">
+        <v>107.3512925</v>
+      </c>
+      <c r="C209" t="n">
+        <v>10.7313672</v>
       </c>
     </row>
     <row r="210">
@@ -2947,10 +3160,11 @@
           <t>Cửa Hàng Sắt Thép Xd Ngọc Lễ</t>
         </is>
       </c>
-      <c r="B210" t="inlineStr">
-        <is>
-          <t>107.3435336,10.7628431,0</t>
-        </is>
+      <c r="B210" t="n">
+        <v>107.3435336</v>
+      </c>
+      <c r="C210" t="n">
+        <v>10.7628431</v>
       </c>
     </row>
     <row r="211">
@@ -2959,10 +3173,11 @@
           <t>Nhà máy tôn thép Sông Ray</t>
         </is>
       </c>
-      <c r="B211" t="inlineStr">
-        <is>
-          <t>107.3505794,10.7674905,0</t>
-        </is>
+      <c r="B211" t="n">
+        <v>107.3505794</v>
+      </c>
+      <c r="C211" t="n">
+        <v>10.7674905</v>
       </c>
     </row>
     <row r="212">
@@ -2971,10 +3186,11 @@
           <t>VLXD Vật Liệu Xây Dựng - Nhà Máy Tôn BẢO BÌNH (chi nhánh 2)</t>
         </is>
       </c>
-      <c r="B212" t="inlineStr">
-        <is>
-          <t>107.3052122,10.7559752,0</t>
-        </is>
+      <c r="B212" t="n">
+        <v>107.3052122</v>
+      </c>
+      <c r="C212" t="n">
+        <v>10.7559752</v>
       </c>
     </row>
     <row r="213">
@@ -2983,10 +3199,11 @@
           <t>Vật liệu xây dựng Năm Tình</t>
         </is>
       </c>
-      <c r="B213" t="inlineStr">
-        <is>
-          <t>107.3769445,10.6169226,0</t>
-        </is>
+      <c r="B213" t="n">
+        <v>107.3769445</v>
+      </c>
+      <c r="C213" t="n">
+        <v>10.6169226</v>
       </c>
     </row>
     <row r="214">
@@ -2995,10 +3212,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Thành Vân</t>
         </is>
       </c>
-      <c r="B214" t="inlineStr">
-        <is>
-          <t>107.5447737,10.5599085,0</t>
-        </is>
+      <c r="B214" t="n">
+        <v>107.5447737</v>
+      </c>
+      <c r="C214" t="n">
+        <v>10.5599085</v>
       </c>
     </row>
     <row r="215">
@@ -3007,10 +3225,11 @@
           <t>Công Ty TNHH Vật Liệu Xây Dựng Tiến Phát</t>
         </is>
       </c>
-      <c r="B215" t="inlineStr">
-        <is>
-          <t>107.4345624,10.5483184,0</t>
-        </is>
+      <c r="B215" t="n">
+        <v>107.4345624</v>
+      </c>
+      <c r="C215" t="n">
+        <v>10.5483184</v>
       </c>
     </row>
     <row r="216">
@@ -3019,10 +3238,11 @@
           <t>Vật Liệu Xây Dựng Nhật Duật</t>
         </is>
       </c>
-      <c r="B216" t="inlineStr">
-        <is>
-          <t>107.3820486,10.8409555,0</t>
-        </is>
+      <c r="B216" t="n">
+        <v>107.3820486</v>
+      </c>
+      <c r="C216" t="n">
+        <v>10.8409555</v>
       </c>
     </row>
     <row r="217">
@@ -3031,10 +3251,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Xuân Hùng</t>
         </is>
       </c>
-      <c r="B217" t="inlineStr">
-        <is>
-          <t>107.2201762,10.7914837,0</t>
-        </is>
+      <c r="B217" t="n">
+        <v>107.2201762</v>
+      </c>
+      <c r="C217" t="n">
+        <v>10.7914837</v>
       </c>
     </row>
     <row r="218">
@@ -3043,10 +3264,11 @@
           <t>VLXD ÁNH</t>
         </is>
       </c>
-      <c r="B218" t="inlineStr">
-        <is>
-          <t>107.1871233,10.8131679,0</t>
-        </is>
+      <c r="B218" t="n">
+        <v>107.1871233</v>
+      </c>
+      <c r="C218" t="n">
+        <v>10.8131679</v>
       </c>
     </row>
     <row r="219">
@@ -3055,10 +3277,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Phong Diễm</t>
         </is>
       </c>
-      <c r="B219" t="inlineStr">
-        <is>
-          <t>107.280003,10.872092,0</t>
-        </is>
+      <c r="B219" t="n">
+        <v>107.280003</v>
+      </c>
+      <c r="C219" t="n">
+        <v>10.872092</v>
       </c>
     </row>
     <row r="220">
@@ -3067,10 +3290,11 @@
           <t>Cửa Hàng VLXD Hiển Xuân</t>
         </is>
       </c>
-      <c r="B220" t="inlineStr">
-        <is>
-          <t>107.1602683,10.8612799,0</t>
-        </is>
+      <c r="B220" t="n">
+        <v>107.1602683</v>
+      </c>
+      <c r="C220" t="n">
+        <v>10.8612799</v>
       </c>
     </row>
     <row r="221">
@@ -3079,10 +3303,11 @@
           <t>Cửa Hàng Vlxd Toàn Thiện</t>
         </is>
       </c>
-      <c r="B221" t="inlineStr">
-        <is>
-          <t>107.2366997,10.8358981,0</t>
-        </is>
+      <c r="B221" t="n">
+        <v>107.2366997</v>
+      </c>
+      <c r="C221" t="n">
+        <v>10.8358981</v>
       </c>
     </row>
     <row r="222">
@@ -3091,10 +3316,11 @@
           <t>Vlxd gạch ốp lát - Lục phát</t>
         </is>
       </c>
-      <c r="B222" t="inlineStr">
-        <is>
-          <t>107.2304671,10.8196677,0</t>
-        </is>
+      <c r="B222" t="n">
+        <v>107.2304671</v>
+      </c>
+      <c r="C222" t="n">
+        <v>10.8196677</v>
       </c>
     </row>
     <row r="223">
@@ -3103,10 +3329,11 @@
           <t>VLXD Gạch Ốp Lát TBVS Phú Gia Home</t>
         </is>
       </c>
-      <c r="B223" t="inlineStr">
-        <is>
-          <t>107.229674,10.8176567,0</t>
-        </is>
+      <c r="B223" t="n">
+        <v>107.229674</v>
+      </c>
+      <c r="C223" t="n">
+        <v>10.8176567</v>
       </c>
     </row>
     <row r="224">
@@ -3115,10 +3342,11 @@
           <t>Cửa Hàng VLXD Lam Anh</t>
         </is>
       </c>
-      <c r="B224" t="inlineStr">
-        <is>
-          <t>107.2325322,10.8244654,0</t>
-        </is>
+      <c r="B224" t="n">
+        <v>107.2325322</v>
+      </c>
+      <c r="C224" t="n">
+        <v>10.8244654</v>
       </c>
     </row>
     <row r="225">
@@ -3127,10 +3355,11 @@
           <t>Cửa Hàng VLXD và Phân Bón - Tấn Thi</t>
         </is>
       </c>
-      <c r="B225" t="inlineStr">
-        <is>
-          <t>107.2794317,10.6968518,0</t>
-        </is>
+      <c r="B225" t="n">
+        <v>107.2794317</v>
+      </c>
+      <c r="C225" t="n">
+        <v>10.6968518</v>
       </c>
     </row>
     <row r="226">
@@ -3139,10 +3368,11 @@
           <t>Cửa hàng Điện-Nước-Đồ sắt Thảo Linh, Xà Bang.</t>
         </is>
       </c>
-      <c r="B226" t="inlineStr">
-        <is>
-          <t>107.2416711,10.7222181,0</t>
-        </is>
+      <c r="B226" t="n">
+        <v>107.2416711</v>
+      </c>
+      <c r="C226" t="n">
+        <v>10.7222181</v>
       </c>
     </row>
     <row r="227">
@@ -3151,10 +3381,11 @@
           <t>Vật liệu xây dựng Bảo Anh</t>
         </is>
       </c>
-      <c r="B227" t="inlineStr">
-        <is>
-          <t>107.2353122,10.7555388,0</t>
-        </is>
+      <c r="B227" t="n">
+        <v>107.2353122</v>
+      </c>
+      <c r="C227" t="n">
+        <v>10.7555388</v>
       </c>
     </row>
     <row r="228">
@@ -3163,10 +3394,11 @@
           <t>Vật liệu xây dựng Tiến Phát</t>
         </is>
       </c>
-      <c r="B228" t="inlineStr">
-        <is>
-          <t>107.2386992,10.7024193,0</t>
-        </is>
+      <c r="B228" t="n">
+        <v>107.2386992</v>
+      </c>
+      <c r="C228" t="n">
+        <v>10.7024193</v>
       </c>
     </row>
     <row r="229">
@@ -3175,10 +3407,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Nguyễn Văn Niệm</t>
         </is>
       </c>
-      <c r="B229" t="inlineStr">
-        <is>
-          <t>107.2419092,10.6312717,0</t>
-        </is>
+      <c r="B229" t="n">
+        <v>107.2419092</v>
+      </c>
+      <c r="C229" t="n">
+        <v>10.6312717</v>
       </c>
     </row>
     <row r="230">
@@ -3187,10 +3420,11 @@
           <t>Công Ty Cp Gạch Ngói Gốm Xd Mỹ Xuân</t>
         </is>
       </c>
-      <c r="B230" t="inlineStr">
-        <is>
-          <t>107.0796279,10.6311929,0</t>
-        </is>
+      <c r="B230" t="n">
+        <v>107.0796279</v>
+      </c>
+      <c r="C230" t="n">
+        <v>10.6311929</v>
       </c>
     </row>
     <row r="231">
@@ -3199,10 +3433,11 @@
           <t>VLXD Minh Phát</t>
         </is>
       </c>
-      <c r="B231" t="inlineStr">
-        <is>
-          <t>107.0615091,10.6270311,0</t>
-        </is>
+      <c r="B231" t="n">
+        <v>107.0615091</v>
+      </c>
+      <c r="C231" t="n">
+        <v>10.6270311</v>
       </c>
     </row>
     <row r="232">
@@ -3211,10 +3446,11 @@
           <t>Cơ sở Mộ Bia Quý</t>
         </is>
       </c>
-      <c r="B232" t="inlineStr">
-        <is>
-          <t>107.2035956,10.7406097,0</t>
-        </is>
+      <c r="B232" t="n">
+        <v>107.2035956</v>
+      </c>
+      <c r="C232" t="n">
+        <v>10.7406097</v>
       </c>
     </row>
     <row r="233">
@@ -3223,10 +3459,11 @@
           <t>Cù Bị</t>
         </is>
       </c>
-      <c r="B233" t="inlineStr">
-        <is>
-          <t>107.1602683,10.7308282,0</t>
-        </is>
+      <c r="B233" t="n">
+        <v>107.1602683</v>
+      </c>
+      <c r="C233" t="n">
+        <v>10.7308282</v>
       </c>
     </row>
     <row r="234">
@@ -3235,10 +3472,11 @@
           <t>VLXD Hùng Phú</t>
         </is>
       </c>
-      <c r="B234" t="inlineStr">
-        <is>
-          <t>107.151058,10.7237625,0</t>
-        </is>
+      <c r="B234" t="n">
+        <v>107.151058</v>
+      </c>
+      <c r="C234" t="n">
+        <v>10.7237625</v>
       </c>
     </row>
     <row r="235">
@@ -3247,10 +3485,11 @@
           <t>Chợ Cù Bị 3</t>
         </is>
       </c>
-      <c r="B235" t="inlineStr">
-        <is>
-          <t>107.1535451,10.7193184,0</t>
-        </is>
+      <c r="B235" t="n">
+        <v>107.1535451</v>
+      </c>
+      <c r="C235" t="n">
+        <v>10.7193184</v>
       </c>
     </row>
     <row r="236">
@@ -3259,10 +3498,11 @@
           <t>Chú cường sông nhạn</t>
         </is>
       </c>
-      <c r="B236" t="inlineStr">
-        <is>
-          <t>107.1327856,10.8292514,0</t>
-        </is>
+      <c r="B236" t="n">
+        <v>107.1327856</v>
+      </c>
+      <c r="C236" t="n">
+        <v>10.8292514</v>
       </c>
     </row>
     <row r="237">
@@ -3271,10 +3511,11 @@
           <t>Công ty Trường Lực</t>
         </is>
       </c>
-      <c r="B237" t="inlineStr">
-        <is>
-          <t>107.0845808,10.8172288,0</t>
-        </is>
+      <c r="B237" t="n">
+        <v>107.0845808</v>
+      </c>
+      <c r="C237" t="n">
+        <v>10.8172288</v>
       </c>
     </row>
     <row r="238">
@@ -3283,10 +3524,11 @@
           <t>Xây dựng Sáu Hiền</t>
         </is>
       </c>
-      <c r="B238" t="inlineStr">
-        <is>
-          <t>107.0378263,10.9982017,0</t>
-        </is>
+      <c r="B238" t="n">
+        <v>107.0378263</v>
+      </c>
+      <c r="C238" t="n">
+        <v>10.9982017</v>
       </c>
     </row>
     <row r="239">
@@ -3295,10 +3537,11 @@
           <t>dgtp bảo bình</t>
         </is>
       </c>
-      <c r="B239" t="inlineStr">
-        <is>
-          <t>107.3122636,10.8075579,0</t>
-        </is>
+      <c r="B239" t="n">
+        <v>107.3122636</v>
+      </c>
+      <c r="C239" t="n">
+        <v>10.8075579</v>
       </c>
     </row>
     <row r="240">
@@ -3307,10 +3550,11 @@
           <t>Bảo Bình</t>
         </is>
       </c>
-      <c r="B240" t="inlineStr">
-        <is>
-          <t>107.2961953,10.8154406,0</t>
-        </is>
+      <c r="B240" t="n">
+        <v>107.2961953</v>
+      </c>
+      <c r="C240" t="n">
+        <v>10.8154406</v>
       </c>
     </row>
     <row r="241">
@@ -3319,10 +3563,11 @@
           <t>VLXD Vật Liệu Xây Dựng BẢO BÌNH (kho Vật liệu)</t>
         </is>
       </c>
-      <c r="B241" t="inlineStr">
-        <is>
-          <t>107.297035,10.83496,0</t>
-        </is>
+      <c r="B241" t="n">
+        <v>107.297035</v>
+      </c>
+      <c r="C241" t="n">
+        <v>10.83496</v>
       </c>
     </row>
     <row r="242">
@@ -3331,10 +3576,11 @@
           <t>Công Ty TNHH Một Thành Viên Xây Dựng Bảo Khánh</t>
         </is>
       </c>
-      <c r="B242" t="inlineStr">
-        <is>
-          <t>107.2838081,10.9029564,0</t>
-        </is>
+      <c r="B242" t="n">
+        <v>107.2838081</v>
+      </c>
+      <c r="C242" t="n">
+        <v>10.9029564</v>
       </c>
     </row>
     <row r="243">
@@ -3343,10 +3589,11 @@
           <t>VLXD Nguyễn Thắng</t>
         </is>
       </c>
-      <c r="B243" t="inlineStr">
-        <is>
-          <t>107.3682,10.762578,0</t>
-        </is>
+      <c r="B243" t="n">
+        <v>107.3682</v>
+      </c>
+      <c r="C243" t="n">
+        <v>10.762578</v>
       </c>
     </row>
     <row r="244">
@@ -3355,10 +3602,11 @@
           <t>VLXD Xe Cuốc Linh Thảo</t>
         </is>
       </c>
-      <c r="B244" t="inlineStr">
-        <is>
-          <t>107.332729,10.7147962,0</t>
-        </is>
+      <c r="B244" t="n">
+        <v>107.332729</v>
+      </c>
+      <c r="C244" t="n">
+        <v>10.7147962</v>
       </c>
     </row>
     <row r="245">
@@ -3367,10 +3615,11 @@
           <t>Vật liệu xây dựng thảo linh</t>
         </is>
       </c>
-      <c r="B245" t="inlineStr">
-        <is>
-          <t>107.3257545,10.6997304,0</t>
-        </is>
+      <c r="B245" t="n">
+        <v>107.3257545</v>
+      </c>
+      <c r="C245" t="n">
+        <v>10.6997304</v>
       </c>
     </row>
     <row r="246">
@@ -3379,10 +3628,11 @@
           <t>VLXD BÁU VINH</t>
         </is>
       </c>
-      <c r="B246" t="inlineStr">
-        <is>
-          <t>107.312364,10.67906,0</t>
-        </is>
+      <c r="B246" t="n">
+        <v>107.312364</v>
+      </c>
+      <c r="C246" t="n">
+        <v>10.67906</v>
       </c>
     </row>
     <row r="247">
@@ -3391,10 +3641,11 @@
           <t>Công ty trách nhiệm hữu hạn san lấp xây dựng Sinh Lộc 68</t>
         </is>
       </c>
-      <c r="B247" t="inlineStr">
-        <is>
-          <t>107.3407015,10.7179792,0</t>
-        </is>
+      <c r="B247" t="n">
+        <v>107.3407015</v>
+      </c>
+      <c r="C247" t="n">
+        <v>10.7179792</v>
       </c>
     </row>
     <row r="248">
@@ -3403,10 +3654,11 @@
           <t>Cửa Hàng Sắt Thép-Tôn Hiếu Điệp</t>
         </is>
       </c>
-      <c r="B248" t="inlineStr">
-        <is>
-          <t>107.335783,10.7194243,0</t>
-        </is>
+      <c r="B248" t="n">
+        <v>107.335783</v>
+      </c>
+      <c r="C248" t="n">
+        <v>10.7194243</v>
       </c>
     </row>
     <row r="249">
@@ -3415,10 +3667,11 @@
           <t>Cơ khí xây dựng Mạnh Hòa Phát</t>
         </is>
       </c>
-      <c r="B249" t="inlineStr">
-        <is>
-          <t>107.3831592,10.7654198,0</t>
-        </is>
+      <c r="B249" t="n">
+        <v>107.3831592</v>
+      </c>
+      <c r="C249" t="n">
+        <v>10.7654198</v>
       </c>
     </row>
     <row r="250">
@@ -3427,10 +3680,11 @@
           <t>CTY XÂY DỰNG &amp; KỸ THUẬT AN PHÚ</t>
         </is>
       </c>
-      <c r="B250" t="inlineStr">
-        <is>
-          <t>107.3296301,10.7430198,0</t>
-        </is>
+      <c r="B250" t="n">
+        <v>107.3296301</v>
+      </c>
+      <c r="C250" t="n">
+        <v>10.7430198</v>
       </c>
     </row>
     <row r="251">
@@ -3439,10 +3693,11 @@
           <t>ay dung le minh</t>
         </is>
       </c>
-      <c r="B251" t="inlineStr">
-        <is>
-          <t>107.2914044,10.7994599,0</t>
-        </is>
+      <c r="B251" t="n">
+        <v>107.2914044</v>
+      </c>
+      <c r="C251" t="n">
+        <v>10.7994599</v>
       </c>
     </row>
     <row r="252">
@@ -3451,10 +3706,11 @@
           <t>Công Ty TNHH Tư Vấn Thiết Kế Và Xây Dựng AnHouse</t>
         </is>
       </c>
-      <c r="B252" t="inlineStr">
-        <is>
-          <t>107.3250732,10.7692567,0</t>
-        </is>
+      <c r="B252" t="n">
+        <v>107.3250732</v>
+      </c>
+      <c r="C252" t="n">
+        <v>10.7692567</v>
       </c>
     </row>
     <row r="253">
@@ -3463,10 +3719,11 @@
           <t>Điện Nước</t>
         </is>
       </c>
-      <c r="B253" t="inlineStr">
-        <is>
-          <t>107.365823,10.8321343,0</t>
-        </is>
+      <c r="B253" t="n">
+        <v>107.365823</v>
+      </c>
+      <c r="C253" t="n">
+        <v>10.8321343</v>
       </c>
     </row>
     <row r="254">
@@ -3475,10 +3732,11 @@
           <t>Nhà thầu xây dựng Mr. Phong</t>
         </is>
       </c>
-      <c r="B254" t="inlineStr">
-        <is>
-          <t>107.3500666,10.827203,0</t>
-        </is>
+      <c r="B254" t="n">
+        <v>107.3500666</v>
+      </c>
+      <c r="C254" t="n">
+        <v>10.827203</v>
       </c>
     </row>
     <row r="255">
@@ -3487,10 +3745,11 @@
           <t>Công Ty Xây Dựng Toàn Bảo Long</t>
         </is>
       </c>
-      <c r="B255" t="inlineStr">
-        <is>
-          <t>107.2939555,10.827611,0</t>
-        </is>
+      <c r="B255" t="n">
+        <v>107.2939555</v>
+      </c>
+      <c r="C255" t="n">
+        <v>10.827611</v>
       </c>
     </row>
     <row r="256">
@@ -3499,10 +3758,11 @@
           <t>Công Ty TNHH Tư Vấn Thiết Kế Mỹ Thuật Xây Dựng Đại Phú Hưng</t>
         </is>
       </c>
-      <c r="B256" t="inlineStr">
-        <is>
-          <t>107.10463,10.7884175,0</t>
-        </is>
+      <c r="B256" t="n">
+        <v>107.10463</v>
+      </c>
+      <c r="C256" t="n">
+        <v>10.7884175</v>
       </c>
     </row>
     <row r="257">
@@ -3511,10 +3771,11 @@
           <t>VLXD Quốc Vệ</t>
         </is>
       </c>
-      <c r="B257" t="inlineStr">
-        <is>
-          <t>107.3888043,10.6855424,0</t>
-        </is>
+      <c r="B257" t="n">
+        <v>107.3888043</v>
+      </c>
+      <c r="C257" t="n">
+        <v>10.6855424</v>
       </c>
     </row>
     <row r="258">
@@ -3523,10 +3784,11 @@
           <t>Công Ty Hiếu Láng</t>
         </is>
       </c>
-      <c r="B258" t="inlineStr">
-        <is>
-          <t>107.2210231,10.7281704,0</t>
-        </is>
+      <c r="B258" t="n">
+        <v>107.2210231</v>
+      </c>
+      <c r="C258" t="n">
+        <v>10.7281704</v>
       </c>
     </row>
     <row r="259">
@@ -3535,10 +3797,11 @@
           <t>Công ty Cổ phần Đo đạc - Xây dựng An Thịnh Phát</t>
         </is>
       </c>
-      <c r="B259" t="inlineStr">
-        <is>
-          <t>107.1958491,10.6897536,0</t>
-        </is>
+      <c r="B259" t="n">
+        <v>107.1958491</v>
+      </c>
+      <c r="C259" t="n">
+        <v>10.6897536</v>
       </c>
     </row>
     <row r="260">
@@ -3547,10 +3810,11 @@
           <t>Bảo liên Giấy Dán Tường</t>
         </is>
       </c>
-      <c r="B260" t="inlineStr">
-        <is>
-          <t>107.1746567,10.680433,0</t>
-        </is>
+      <c r="B260" t="n">
+        <v>107.1746567</v>
+      </c>
+      <c r="C260" t="n">
+        <v>10.680433</v>
       </c>
     </row>
     <row r="261">
@@ -3559,10 +3823,11 @@
           <t>CÔNG TY TNHH XD THÀNH ĐẠT PHÁT</t>
         </is>
       </c>
-      <c r="B261" t="inlineStr">
-        <is>
-          <t>107.1782244,10.6571601,0</t>
-        </is>
+      <c r="B261" t="n">
+        <v>107.1782244</v>
+      </c>
+      <c r="C261" t="n">
+        <v>10.6571601</v>
       </c>
     </row>
     <row r="262">
@@ -3571,10 +3836,11 @@
           <t>Nhà thầu xây dựng - Nguyễn Văn Phúc</t>
         </is>
       </c>
-      <c r="B262" t="inlineStr">
-        <is>
-          <t>107.1839014,10.7295069,0</t>
-        </is>
+      <c r="B262" t="n">
+        <v>107.1839014</v>
+      </c>
+      <c r="C262" t="n">
+        <v>10.7295069</v>
       </c>
     </row>
     <row r="263">
@@ -3583,10 +3849,11 @@
           <t>Nhà Thầu Xây Dựng ThaiCons - Vật Liệu Xây Dựng</t>
         </is>
       </c>
-      <c r="B263" t="inlineStr">
-        <is>
-          <t>107.2004521,10.5933867,0</t>
-        </is>
+      <c r="B263" t="n">
+        <v>107.2004521</v>
+      </c>
+      <c r="C263" t="n">
+        <v>10.5933867</v>
       </c>
     </row>
     <row r="264">
@@ -3595,10 +3862,11 @@
           <t>Xây Dựng - sửa chữa dân dụng Minh Dũng</t>
         </is>
       </c>
-      <c r="B264" t="inlineStr">
-        <is>
-          <t>107.1792863,10.5851787,0</t>
-        </is>
+      <c r="B264" t="n">
+        <v>107.1792863</v>
+      </c>
+      <c r="C264" t="n">
+        <v>10.5851787</v>
       </c>
     </row>
     <row r="265">
@@ -3607,10 +3875,11 @@
           <t>Công Ty Cổ Phần Vật Liệu Xây Dựng Dic</t>
         </is>
       </c>
-      <c r="B265" t="inlineStr">
-        <is>
-          <t>107.1644102,10.5546011,0</t>
-        </is>
+      <c r="B265" t="n">
+        <v>107.1644102</v>
+      </c>
+      <c r="C265" t="n">
+        <v>10.5546011</v>
       </c>
     </row>
     <row r="266">
@@ -3619,10 +3888,11 @@
           <t>Công ty Xây Dựng Nguyễn Đình - Nhà Xanh Xuân Lộc</t>
         </is>
       </c>
-      <c r="B266" t="inlineStr">
-        <is>
-          <t>107.4020519,10.9177465,0</t>
-        </is>
+      <c r="B266" t="n">
+        <v>107.4020519</v>
+      </c>
+      <c r="C266" t="n">
+        <v>10.9177465</v>
       </c>
     </row>
     <row r="267">
@@ -3631,10 +3901,11 @@
           <t>Vật liệu xây dựng Gia Học</t>
         </is>
       </c>
-      <c r="B267" t="inlineStr">
-        <is>
-          <t>107.2610413,10.9208467,0</t>
-        </is>
+      <c r="B267" t="n">
+        <v>107.2610413</v>
+      </c>
+      <c r="C267" t="n">
+        <v>10.9208467</v>
       </c>
     </row>
     <row r="268">
@@ -3643,10 +3914,11 @@
           <t>Vật Liệu Xây Dựng Xuân Tân - Long Khánh - Đồng Nai</t>
         </is>
       </c>
-      <c r="B268" t="inlineStr">
-        <is>
-          <t>107.2338276,10.9080052,0</t>
-        </is>
+      <c r="B268" t="n">
+        <v>107.2338276</v>
+      </c>
+      <c r="C268" t="n">
+        <v>10.9080052</v>
       </c>
     </row>
     <row r="269">
@@ -3655,10 +3927,11 @@
           <t>Cửa hàng VLXD Trang Trí Nội Thất Lộc Phát</t>
         </is>
       </c>
-      <c r="B269" t="inlineStr">
-        <is>
-          <t>107.2431245,10.921396,0</t>
-        </is>
+      <c r="B269" t="n">
+        <v>107.2431245</v>
+      </c>
+      <c r="C269" t="n">
+        <v>10.921396</v>
       </c>
     </row>
     <row r="270">
@@ -3667,10 +3940,11 @@
           <t>Công Ty TNHH VLXD THANH</t>
         </is>
       </c>
-      <c r="B270" t="inlineStr">
-        <is>
-          <t>107.2392042,10.937315,0</t>
-        </is>
+      <c r="B270" t="n">
+        <v>107.2392042</v>
+      </c>
+      <c r="C270" t="n">
+        <v>10.937315</v>
       </c>
     </row>
     <row r="271">
@@ -3679,10 +3953,11 @@
           <t>Cửa Hàng VLXD Hoàng</t>
         </is>
       </c>
-      <c r="B271" t="inlineStr">
-        <is>
-          <t>107.2580737,10.9462977,0</t>
-        </is>
+      <c r="B271" t="n">
+        <v>107.2580737</v>
+      </c>
+      <c r="C271" t="n">
+        <v>10.9462977</v>
       </c>
     </row>
     <row r="272">
@@ -3691,10 +3966,11 @@
           <t>VLXD ÚT TÂN</t>
         </is>
       </c>
-      <c r="B272" t="inlineStr">
-        <is>
-          <t>107.241535,10.9561456,0</t>
-        </is>
+      <c r="B272" t="n">
+        <v>107.241535</v>
+      </c>
+      <c r="C272" t="n">
+        <v>10.9561456</v>
       </c>
     </row>
     <row r="273">
@@ -3703,10 +3979,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Chiến</t>
         </is>
       </c>
-      <c r="B273" t="inlineStr">
-        <is>
-          <t>107.2716479,10.9425824,0</t>
-        </is>
+      <c r="B273" t="n">
+        <v>107.2716479</v>
+      </c>
+      <c r="C273" t="n">
+        <v>10.9425824</v>
       </c>
     </row>
     <row r="274">
@@ -3715,10 +3992,11 @@
           <t>VLXD Thanh Long Khánh ( Showroom TLK - Quốc Tâm)</t>
         </is>
       </c>
-      <c r="B274" t="inlineStr">
-        <is>
-          <t>107.2421288,10.9409775,0</t>
-        </is>
+      <c r="B274" t="n">
+        <v>107.2421288</v>
+      </c>
+      <c r="C274" t="n">
+        <v>10.9409775</v>
       </c>
     </row>
     <row r="275">
@@ -3727,10 +4005,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng &amp; Trang Trí Nội Thất Biển Hà</t>
         </is>
       </c>
-      <c r="B275" t="inlineStr">
-        <is>
-          <t>107.2426289,10.9292567,0</t>
-        </is>
+      <c r="B275" t="n">
+        <v>107.2426289</v>
+      </c>
+      <c r="C275" t="n">
+        <v>10.9292567</v>
       </c>
     </row>
     <row r="276">
@@ -3739,10 +4018,11 @@
           <t>CÔNG TY TNHH XÂY DỰNG NGỌC ĐĂNG KHOA</t>
         </is>
       </c>
-      <c r="B276" t="inlineStr">
-        <is>
-          <t>107.2584918,10.9189876,0</t>
-        </is>
+      <c r="B276" t="n">
+        <v>107.2584918</v>
+      </c>
+      <c r="C276" t="n">
+        <v>10.9189876</v>
       </c>
     </row>
     <row r="277">
@@ -3751,10 +4031,11 @@
           <t>Cty TNHH Thiết Kế Xây Dựng Nét Đẹp Việt</t>
         </is>
       </c>
-      <c r="B277" t="inlineStr">
-        <is>
-          <t>107.2479385,10.923224,0</t>
-        </is>
+      <c r="B277" t="n">
+        <v>107.2479385</v>
+      </c>
+      <c r="C277" t="n">
+        <v>10.923224</v>
       </c>
     </row>
     <row r="278">
@@ -3763,10 +4044,11 @@
           <t>Thiết kế xây dựng Long Khánh - Hachi Home</t>
         </is>
       </c>
-      <c r="B278" t="inlineStr">
-        <is>
-          <t>107.2392332,10.922208,0</t>
-        </is>
+      <c r="B278" t="n">
+        <v>107.2392332</v>
+      </c>
+      <c r="C278" t="n">
+        <v>10.922208</v>
       </c>
     </row>
     <row r="279">
@@ -3775,10 +4057,11 @@
           <t>Công ty TNHH Tư vấn Khảo sát và Xây dựng Tân Tiến ( Đo đạc Đồng Nai)</t>
         </is>
       </c>
-      <c r="B279" t="inlineStr">
-        <is>
-          <t>107.2472046,10.9284834,0</t>
-        </is>
+      <c r="B279" t="n">
+        <v>107.2472046</v>
+      </c>
+      <c r="C279" t="n">
+        <v>10.9284834</v>
       </c>
     </row>
     <row r="280">
@@ -3787,10 +4070,11 @@
           <t>CTY TNHH THIẾT KẾ - XÂY DỰNG NGUYỄN BẢY</t>
         </is>
       </c>
-      <c r="B280" t="inlineStr">
-        <is>
-          <t>107.2561016,10.9404308,0</t>
-        </is>
+      <c r="B280" t="n">
+        <v>107.2561016</v>
+      </c>
+      <c r="C280" t="n">
+        <v>10.9404308</v>
       </c>
     </row>
     <row r="281">
@@ -3799,10 +4083,11 @@
           <t>CÔNG TY TNHH THIẾT KẾ ĐẦU TƯ XÂY DỰNG HÙNG ANH</t>
         </is>
       </c>
-      <c r="B281" t="inlineStr">
-        <is>
-          <t>107.2440003,10.9407793,0</t>
-        </is>
+      <c r="B281" t="n">
+        <v>107.2440003</v>
+      </c>
+      <c r="C281" t="n">
+        <v>10.9407793</v>
       </c>
     </row>
     <row r="282">
@@ -3811,10 +4096,11 @@
           <t>CÔNG TY TNHH XÂY DỰNG VÀ ĐẦU TƯ WINCONS - CN1</t>
         </is>
       </c>
-      <c r="B282" t="inlineStr">
-        <is>
-          <t>107.2428219,10.9454365,0</t>
-        </is>
+      <c r="B282" t="n">
+        <v>107.2428219</v>
+      </c>
+      <c r="C282" t="n">
+        <v>10.9454365</v>
       </c>
     </row>
     <row r="283">
@@ -3823,10 +4109,11 @@
           <t>Công Ty TNHH Đầu Tư và Phát Triển Xây Dựng Phong Vũ</t>
         </is>
       </c>
-      <c r="B283" t="inlineStr">
-        <is>
-          <t>107.2459412,10.6485699,0</t>
-        </is>
+      <c r="B283" t="n">
+        <v>107.2459412</v>
+      </c>
+      <c r="C283" t="n">
+        <v>10.6485699</v>
       </c>
     </row>
     <row r="284">
@@ -3835,10 +4122,11 @@
           <t>Công Ty Cổ Phần Xây Dựng Và Phát Triển Đô Thị Châu Đức</t>
         </is>
       </c>
-      <c r="B284" t="inlineStr">
-        <is>
-          <t>107.2408946,10.6486074,0</t>
-        </is>
+      <c r="B284" t="n">
+        <v>107.2408946</v>
+      </c>
+      <c r="C284" t="n">
+        <v>10.6486074</v>
       </c>
     </row>
     <row r="285">
@@ -3847,10 +4135,11 @@
           <t>Công ty Cổ phần Xây dựng Thương mại Nhật Nam</t>
         </is>
       </c>
-      <c r="B285" t="inlineStr">
-        <is>
-          <t>107.2386744,10.6492456,0</t>
-        </is>
+      <c r="B285" t="n">
+        <v>107.2386744</v>
+      </c>
+      <c r="C285" t="n">
+        <v>10.6492456</v>
       </c>
     </row>
     <row r="286">
@@ -3859,10 +4148,11 @@
           <t>Cơ Khí Xây Dựng Nhật</t>
         </is>
       </c>
-      <c r="B286" t="inlineStr">
-        <is>
-          <t>107.2434505,10.6388149,0</t>
-        </is>
+      <c r="B286" t="n">
+        <v>107.2434505</v>
+      </c>
+      <c r="C286" t="n">
+        <v>10.6388149</v>
       </c>
     </row>
     <row r="287">
@@ -3871,10 +4161,11 @@
           <t>Công Ty TNHH Một Thành Viên Thép Quốc Dũng</t>
         </is>
       </c>
-      <c r="B287" t="inlineStr">
-        <is>
-          <t>107.455218,10.8665318,0</t>
-        </is>
+      <c r="B287" t="n">
+        <v>107.455218</v>
+      </c>
+      <c r="C287" t="n">
+        <v>10.8665318</v>
       </c>
     </row>
     <row r="288">
@@ -3883,10 +4174,11 @@
           <t>Cửa Hàng Sắt Thép QUỐC TIẾN</t>
         </is>
       </c>
-      <c r="B288" t="inlineStr">
-        <is>
-          <t>107.3956658,10.9122356,0</t>
-        </is>
+      <c r="B288" t="n">
+        <v>107.3956658</v>
+      </c>
+      <c r="C288" t="n">
+        <v>10.9122356</v>
       </c>
     </row>
     <row r="289">
@@ -3895,10 +4187,11 @@
           <t>Tôn Gia Lễ</t>
         </is>
       </c>
-      <c r="B289" t="inlineStr">
-        <is>
-          <t>107.2765575,10.9008602,0</t>
-        </is>
+      <c r="B289" t="n">
+        <v>107.2765575</v>
+      </c>
+      <c r="C289" t="n">
+        <v>10.9008602</v>
       </c>
     </row>
     <row r="290">
@@ -3907,10 +4200,11 @@
           <t>Công Ty Cp Xây Dựng Cao Su Doruco</t>
         </is>
       </c>
-      <c r="B290" t="inlineStr">
-        <is>
-          <t>107.185294,10.9406493,0</t>
-        </is>
+      <c r="B290" t="n">
+        <v>107.185294</v>
+      </c>
+      <c r="C290" t="n">
+        <v>10.9406493</v>
       </c>
     </row>
     <row r="291">
@@ -3919,10 +4213,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Hùng</t>
         </is>
       </c>
-      <c r="B291" t="inlineStr">
-        <is>
-          <t>107.1918743,10.8719288,0</t>
-        </is>
+      <c r="B291" t="n">
+        <v>107.1918743</v>
+      </c>
+      <c r="C291" t="n">
+        <v>10.8719288</v>
       </c>
     </row>
     <row r="292">
@@ -3931,10 +4226,11 @@
           <t>Xuân Lập</t>
         </is>
       </c>
-      <c r="B292" t="inlineStr">
-        <is>
-          <t>107.1779936,10.9092302,0</t>
-        </is>
+      <c r="B292" t="n">
+        <v>107.1779936</v>
+      </c>
+      <c r="C292" t="n">
+        <v>10.9092302</v>
       </c>
     </row>
     <row r="293">
@@ -3943,10 +4239,11 @@
           <t>Kho Sắt Thép Xuân Thống</t>
         </is>
       </c>
-      <c r="B293" t="inlineStr">
-        <is>
-          <t>107.1839643,10.9301808,0</t>
-        </is>
+      <c r="B293" t="n">
+        <v>107.1839643</v>
+      </c>
+      <c r="C293" t="n">
+        <v>10.9301808</v>
       </c>
     </row>
     <row r="294">
@@ -3955,10 +4252,11 @@
           <t>VLXD Phú Trường Dũng II</t>
         </is>
       </c>
-      <c r="B294" t="inlineStr">
-        <is>
-          <t>107.1874938,10.9248201,0</t>
-        </is>
+      <c r="B294" t="n">
+        <v>107.1874938</v>
+      </c>
+      <c r="C294" t="n">
+        <v>10.9248201</v>
       </c>
     </row>
     <row r="295">
@@ -3967,10 +4265,11 @@
           <t>VHX Xuân Lập</t>
         </is>
       </c>
-      <c r="B295" t="inlineStr">
-        <is>
-          <t>107.185277,10.925613,0</t>
-        </is>
+      <c r="B295" t="n">
+        <v>107.185277</v>
+      </c>
+      <c r="C295" t="n">
+        <v>10.925613</v>
       </c>
     </row>
     <row r="296">
@@ -3979,10 +4278,11 @@
           <t>Cửa Hàng Vlxd Công Thành</t>
         </is>
       </c>
-      <c r="B296" t="inlineStr">
-        <is>
-          <t>107.2295735,10.9013736,0</t>
-        </is>
+      <c r="B296" t="n">
+        <v>107.2295735</v>
+      </c>
+      <c r="C296" t="n">
+        <v>10.9013736</v>
       </c>
     </row>
     <row r="297">
@@ -3991,10 +4291,11 @@
           <t>Cửa Hàng Vật Liệu Xây Dựng Ánh</t>
         </is>
       </c>
-      <c r="B297" t="inlineStr">
-        <is>
-          <t>107.1996238,10.8768876,0</t>
-        </is>
+      <c r="B297" t="n">
+        <v>107.1996238</v>
+      </c>
+      <c r="C297" t="n">
+        <v>10.8768876</v>
       </c>
     </row>
     <row r="298">
@@ -4003,10 +4304,11 @@
           <t>VLXD Minh Tuấn</t>
         </is>
       </c>
-      <c r="B298" t="inlineStr">
-        <is>
-          <t>107.2499741,10.9190686,0</t>
-        </is>
+      <c r="B298" t="n">
+        <v>107.2499741</v>
+      </c>
+      <c r="C298" t="n">
+        <v>10.9190686</v>
       </c>
     </row>
     <row r="299">
@@ -4015,10 +4317,11 @@
           <t>Cửa Hàng Vlxd Bình Minh</t>
         </is>
       </c>
-      <c r="B299" t="inlineStr">
-        <is>
-          <t>107.2321755,10.9057944,0</t>
-        </is>
+      <c r="B299" t="n">
+        <v>107.2321755</v>
+      </c>
+      <c r="C299" t="n">
+        <v>10.9057944</v>
       </c>
     </row>
     <row r="300">
@@ -4027,10 +4330,11 @@
           <t>VLXD Thanh 2</t>
         </is>
       </c>
-      <c r="B300" t="inlineStr">
-        <is>
-          <t>107.237057,10.958172,0</t>
-        </is>
+      <c r="B300" t="n">
+        <v>107.237057</v>
+      </c>
+      <c r="C300" t="n">
+        <v>10.958172</v>
       </c>
     </row>
     <row r="301">
@@ -4039,10 +4343,11 @@
           <t>ATAD Steel Structure Corporation (Dong Nai Factory)</t>
         </is>
       </c>
-      <c r="B301" t="inlineStr">
-        <is>
-          <t>107.2186164,10.9654609,0</t>
-        </is>
+      <c r="B301" t="n">
+        <v>107.2186164</v>
+      </c>
+      <c r="C301" t="n">
+        <v>10.9654609</v>
       </c>
     </row>
     <row r="302">
@@ -4051,10 +4356,11 @@
           <t>Long Giao</t>
         </is>
       </c>
-      <c r="B302" t="inlineStr">
-        <is>
-          <t>107.2282225,10.8274876,0</t>
-        </is>
+      <c r="B302" t="n">
+        <v>107.2282225</v>
+      </c>
+      <c r="C302" t="n">
+        <v>10.8274876</v>
       </c>
     </row>
   </sheetData>

</xml_diff>